<commit_message>
* Updated cleaned 2015 taxation data * New functions in `read_data.py` to import cleaned 2015 taxation data * Updated `map_gini_2015.py` to use new data reading functions
</commit_message>
<xml_diff>
--- a/data/Steuern_Klassen_Wohnviertel_cleaned.xlsx
+++ b/data/Steuern_Klassen_Wohnviertel_cleaned.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17540" activeTab="2"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="2" r:id="rId1"/>
@@ -3348,7 +3348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
@@ -6046,7 +6046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
* Incorporated quintile data into XLSX file * Reverted conda environment name * `read_data.py` now includes functions to read quintile data
</commit_message>
<xml_diff>
--- a/data/Steuern_Klassen_Wohnviertel_cleaned.xlsx
+++ b/data/Steuern_Klassen_Wohnviertel_cleaned.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylan/Development/TaxationInequality_GIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13A0E1D9-8DE4-4C4A-8498-FC7049778809}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17540" activeTab="1"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="2" r:id="rId1"/>
-    <sheet name="Assets" sheetId="5" r:id="rId2"/>
-    <sheet name="mapping_wohnviertel_geo_id" sheetId="7" r:id="rId3"/>
-    <sheet name="mapping_wohnviertel_id" sheetId="3" r:id="rId4"/>
-    <sheet name="mapping_incomeclass_id" sheetId="4" r:id="rId5"/>
-    <sheet name="mapping_assetclass_id" sheetId="6" r:id="rId6"/>
+    <sheet name="Income_quintiles" sheetId="8" r:id="rId2"/>
+    <sheet name="Assets" sheetId="5" r:id="rId3"/>
+    <sheet name="Assets_quintiles" sheetId="9" r:id="rId4"/>
+    <sheet name="mapping_wohnviertel_geo_id" sheetId="7" r:id="rId5"/>
+    <sheet name="mapping_wohnviertel_id" sheetId="3" r:id="rId6"/>
+    <sheet name="mapping_incomeclass_id" sheetId="4" r:id="rId7"/>
+    <sheet name="mapping_assetclass_id" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_AMO_SingleObject_151849305_ROM_F0.SEC2.Tabulate_1.SEC1.BDY.Kreuztabellenbericht_Tabelle_1" hidden="1">#REF!</definedName>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>Altstadt Grossbasel</t>
   </si>
@@ -205,13 +208,21 @@
   <si>
     <t>geo_wohnviertel_id</t>
   </si>
+  <si>
+    <t>incomequintile_id</t>
+  </si>
+  <si>
+    <t>assetquintile_id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -286,12 +297,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -301,11 +313,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 3" xfId="1"/>
+    <cellStyle name="Standard 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -640,11 +654,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G233"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5:B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3345,11 +3359,2288 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA76009E-9503-7840-9C54-03E7EF448422}">
+  <dimension ref="A1:F111"/>
+  <sheetViews>
+    <sheetView zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>335</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1330220</v>
+      </c>
+      <c r="F5" s="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9">
+        <v>335</v>
+      </c>
+      <c r="E6" s="9">
+        <v>6878185</v>
+      </c>
+      <c r="F6" s="9">
+        <v>184671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9">
+        <v>335</v>
+      </c>
+      <c r="E7" s="9">
+        <v>17391161</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2233910</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9">
+        <v>335</v>
+      </c>
+      <c r="E8" s="9">
+        <v>31771183</v>
+      </c>
+      <c r="F8" s="9">
+        <v>5158796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="str">
+        <f>VLOOKUP(A9,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="9">
+        <v>335</v>
+      </c>
+      <c r="E9" s="9">
+        <v>106975586</v>
+      </c>
+      <c r="F9" s="9">
+        <v>20323529</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="str">
+        <f>VLOOKUP(A10,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>600</v>
+      </c>
+      <c r="E10" s="9">
+        <v>4921051</v>
+      </c>
+      <c r="F10" s="9">
+        <v>11375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="str">
+        <f>VLOOKUP(A11,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9">
+        <v>600</v>
+      </c>
+      <c r="E11" s="9">
+        <v>19997280</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1633999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="str">
+        <f>VLOOKUP(A12,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="9">
+        <v>600</v>
+      </c>
+      <c r="E12" s="9">
+        <v>35494307</v>
+      </c>
+      <c r="F12" s="9">
+        <v>4822525</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="str">
+        <f>VLOOKUP(A13,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
+        <v>600</v>
+      </c>
+      <c r="E13" s="9">
+        <v>57914499</v>
+      </c>
+      <c r="F13" s="9">
+        <v>9116508</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="str">
+        <f>VLOOKUP(A14,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9">
+        <v>599</v>
+      </c>
+      <c r="E14" s="9">
+        <v>179840543</v>
+      </c>
+      <c r="F14" s="9">
+        <v>33613224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="str">
+        <f>VLOOKUP(A15,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1248</v>
+      </c>
+      <c r="E15" s="9">
+        <v>8106773</v>
+      </c>
+      <c r="F15" s="9">
+        <v>5851</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1248</v>
+      </c>
+      <c r="E16" s="9">
+        <v>37569684</v>
+      </c>
+      <c r="F16" s="9">
+        <v>2465798</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="str">
+        <f>VLOOKUP(A17,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1248</v>
+      </c>
+      <c r="E17" s="9">
+        <v>66299933</v>
+      </c>
+      <c r="F17" s="9">
+        <v>8228381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="str">
+        <f>VLOOKUP(A18,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1248</v>
+      </c>
+      <c r="E18" s="9">
+        <v>103587213</v>
+      </c>
+      <c r="F18" s="9">
+        <v>15247132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP(A19,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1247</v>
+      </c>
+      <c r="E19" s="9">
+        <v>257605751</v>
+      </c>
+      <c r="F19" s="9">
+        <v>44649403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1100</v>
+      </c>
+      <c r="E20" s="9">
+        <v>10171079</v>
+      </c>
+      <c r="F20" s="9">
+        <v>121398</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP(A21,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1099</v>
+      </c>
+      <c r="E21" s="9">
+        <v>34302426</v>
+      </c>
+      <c r="F21" s="9">
+        <v>2287363</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="str">
+        <f>VLOOKUP(A22,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1100</v>
+      </c>
+      <c r="E22" s="9">
+        <v>52479423</v>
+      </c>
+      <c r="F22" s="9">
+        <v>5838183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="str">
+        <f>VLOOKUP(A23,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1099</v>
+      </c>
+      <c r="E23" s="9">
+        <v>72406787</v>
+      </c>
+      <c r="F23" s="9">
+        <v>9258391</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="str">
+        <f>VLOOKUP(A24,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24" s="9">
+        <v>1099</v>
+      </c>
+      <c r="E24" s="9">
+        <v>140079868</v>
+      </c>
+      <c r="F24" s="9">
+        <v>22557320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="str">
+        <f>VLOOKUP(A25,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1288</v>
+      </c>
+      <c r="E25" s="9">
+        <v>13585356</v>
+      </c>
+      <c r="F25" s="9">
+        <v>203057</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="str">
+        <f>VLOOKUP(A26,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1288</v>
+      </c>
+      <c r="E26" s="9">
+        <v>50062352</v>
+      </c>
+      <c r="F26" s="9">
+        <v>4604127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="str">
+        <f>VLOOKUP(A27,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1288</v>
+      </c>
+      <c r="E27" s="9">
+        <v>79347863</v>
+      </c>
+      <c r="F27" s="9">
+        <v>10312084</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="str">
+        <f>VLOOKUP(A28,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1288</v>
+      </c>
+      <c r="E28" s="9">
+        <v>122156622</v>
+      </c>
+      <c r="F28" s="9">
+        <v>18460576</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" t="str">
+        <f>VLOOKUP(A29,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1287</v>
+      </c>
+      <c r="E29" s="9">
+        <v>381775997</v>
+      </c>
+      <c r="F29" s="9">
+        <v>70654254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="str">
+        <f>VLOOKUP(A30,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="9">
+        <v>2309</v>
+      </c>
+      <c r="E30" s="9">
+        <v>16590609</v>
+      </c>
+      <c r="F30" s="9">
+        <v>42477</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="str">
+        <f>VLOOKUP(A31,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="9">
+        <v>2308</v>
+      </c>
+      <c r="E31" s="9">
+        <v>65496590</v>
+      </c>
+      <c r="F31" s="9">
+        <v>3711308</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="str">
+        <f>VLOOKUP(A32,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" s="9">
+        <v>2308</v>
+      </c>
+      <c r="E32" s="9">
+        <v>109118192</v>
+      </c>
+      <c r="F32" s="9">
+        <v>12100789</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="str">
+        <f>VLOOKUP(A33,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" s="9">
+        <v>2308</v>
+      </c>
+      <c r="E33" s="9">
+        <v>154750091</v>
+      </c>
+      <c r="F33" s="9">
+        <v>20745338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="str">
+        <f>VLOOKUP(A34,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34" s="9">
+        <v>2308</v>
+      </c>
+      <c r="E34" s="9">
+        <v>295434786</v>
+      </c>
+      <c r="F34" s="9">
+        <v>46917663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" t="str">
+        <f>VLOOKUP(A35,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="9">
+        <v>998</v>
+      </c>
+      <c r="E35" s="9">
+        <v>7142525</v>
+      </c>
+      <c r="F35" s="9">
+        <v>34361</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36" t="str">
+        <f>VLOOKUP(A36,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="9">
+        <v>997</v>
+      </c>
+      <c r="E36" s="9">
+        <v>37408668</v>
+      </c>
+      <c r="F36" s="9">
+        <v>3212019</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37" t="str">
+        <f>VLOOKUP(A37,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" s="9">
+        <v>997</v>
+      </c>
+      <c r="E37" s="9">
+        <v>65142548</v>
+      </c>
+      <c r="F37" s="9">
+        <v>8384093</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="str">
+        <f>VLOOKUP(A38,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" s="9">
+        <v>997</v>
+      </c>
+      <c r="E38" s="9">
+        <v>104113396</v>
+      </c>
+      <c r="F38" s="9">
+        <v>15411942</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" t="str">
+        <f>VLOOKUP(A39,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39" s="9">
+        <v>997</v>
+      </c>
+      <c r="E39" s="9">
+        <v>361067225</v>
+      </c>
+      <c r="F39" s="9">
+        <v>71150407</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40" t="str">
+        <f>VLOOKUP(A40,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9">
+        <v>1623</v>
+      </c>
+      <c r="E40" s="9">
+        <v>14448978</v>
+      </c>
+      <c r="F40" s="9">
+        <v>104137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="B41" t="str">
+        <f>VLOOKUP(A41,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="9">
+        <v>1622</v>
+      </c>
+      <c r="E41" s="9">
+        <v>58624753</v>
+      </c>
+      <c r="F41" s="9">
+        <v>4975659</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42" t="str">
+        <f>VLOOKUP(A42,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" s="9">
+        <v>1623</v>
+      </c>
+      <c r="E42" s="9">
+        <v>93991384</v>
+      </c>
+      <c r="F42" s="9">
+        <v>11955320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43" t="str">
+        <f>VLOOKUP(A43,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43" s="9">
+        <v>1622</v>
+      </c>
+      <c r="E43" s="9">
+        <v>137184734</v>
+      </c>
+      <c r="F43" s="9">
+        <v>19360086</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="str">
+        <f>VLOOKUP(A44,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44" s="9">
+        <v>1622</v>
+      </c>
+      <c r="E44" s="9">
+        <v>326685315</v>
+      </c>
+      <c r="F44" s="9">
+        <v>56036600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="str">
+        <f>VLOOKUP(A45,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="9">
+        <v>839</v>
+      </c>
+      <c r="E45" s="9">
+        <v>7447929</v>
+      </c>
+      <c r="F45" s="9">
+        <v>52543</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46" t="str">
+        <f>VLOOKUP(A46,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="9">
+        <v>838</v>
+      </c>
+      <c r="E46" s="9">
+        <v>26913020</v>
+      </c>
+      <c r="F46" s="9">
+        <v>1995433</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47" t="str">
+        <f>VLOOKUP(A47,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" s="9">
+        <v>838</v>
+      </c>
+      <c r="E47" s="9">
+        <v>42900217</v>
+      </c>
+      <c r="F47" s="9">
+        <v>5055150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="B48" t="str">
+        <f>VLOOKUP(A48,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" s="9">
+        <v>838</v>
+      </c>
+      <c r="E48" s="9">
+        <v>62754764</v>
+      </c>
+      <c r="F48" s="9">
+        <v>8648376</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49" t="str">
+        <f>VLOOKUP(A49,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49" s="9">
+        <v>838</v>
+      </c>
+      <c r="E49" s="9">
+        <v>126245302</v>
+      </c>
+      <c r="F49" s="9">
+        <v>20490270</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50" t="str">
+        <f>VLOOKUP(A50,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" s="9">
+        <v>1948</v>
+      </c>
+      <c r="E50" s="9">
+        <v>12501849</v>
+      </c>
+      <c r="F50" s="9">
+        <v>61210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51" t="str">
+        <f>VLOOKUP(A51,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" s="9">
+        <v>1948</v>
+      </c>
+      <c r="E51" s="9">
+        <v>52888728</v>
+      </c>
+      <c r="F51" s="9">
+        <v>2670510</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52" t="str">
+        <f>VLOOKUP(A52,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" s="9">
+        <v>1949</v>
+      </c>
+      <c r="E52" s="9">
+        <v>87356328</v>
+      </c>
+      <c r="F52" s="9">
+        <v>9009274</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53" t="str">
+        <f>VLOOKUP(A53,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53" s="9">
+        <v>1947</v>
+      </c>
+      <c r="E53" s="9">
+        <v>122649538</v>
+      </c>
+      <c r="F53" s="9">
+        <v>15263065</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54" t="str">
+        <f>VLOOKUP(A54,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54" s="9">
+        <v>1947</v>
+      </c>
+      <c r="E54" s="9">
+        <v>228969982</v>
+      </c>
+      <c r="F54" s="9">
+        <v>34511574</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>11</v>
+      </c>
+      <c r="B55" t="str">
+        <f>VLOOKUP(A55,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" s="9">
+        <v>2179</v>
+      </c>
+      <c r="E55" s="9">
+        <v>9261501</v>
+      </c>
+      <c r="F55" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>11</v>
+      </c>
+      <c r="B56" t="str">
+        <f>VLOOKUP(A56,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" s="9">
+        <v>2179</v>
+      </c>
+      <c r="E56" s="9">
+        <v>49753161</v>
+      </c>
+      <c r="F56" s="9">
+        <v>1645353</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>11</v>
+      </c>
+      <c r="B57" t="str">
+        <f>VLOOKUP(A57,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" s="9">
+        <v>2179</v>
+      </c>
+      <c r="E57" s="9">
+        <v>91470270</v>
+      </c>
+      <c r="F57" s="9">
+        <v>8724984</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>11</v>
+      </c>
+      <c r="B58" t="str">
+        <f>VLOOKUP(A58,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" s="9">
+        <v>2179</v>
+      </c>
+      <c r="E58" s="9">
+        <v>135934194</v>
+      </c>
+      <c r="F58" s="9">
+        <v>16556794</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>11</v>
+      </c>
+      <c r="B59" t="str">
+        <f>VLOOKUP(A59,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59" s="9">
+        <v>2178</v>
+      </c>
+      <c r="E59" s="9">
+        <v>283046321</v>
+      </c>
+      <c r="F59" s="9">
+        <v>44800611</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60">
+        <v>12</v>
+      </c>
+      <c r="B60" t="str">
+        <f>VLOOKUP(A60,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" s="9">
+        <v>318</v>
+      </c>
+      <c r="E60" s="9">
+        <v>1339679</v>
+      </c>
+      <c r="F60" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61">
+        <v>12</v>
+      </c>
+      <c r="B61" t="str">
+        <f>VLOOKUP(A61,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" s="9">
+        <v>318</v>
+      </c>
+      <c r="E61" s="9">
+        <v>7147127</v>
+      </c>
+      <c r="F61" s="9">
+        <v>234228</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>12</v>
+      </c>
+      <c r="B62" t="str">
+        <f>VLOOKUP(A62,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" s="9">
+        <v>317</v>
+      </c>
+      <c r="E62" s="9">
+        <v>13473760</v>
+      </c>
+      <c r="F62" s="9">
+        <v>1426677</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>12</v>
+      </c>
+      <c r="B63" t="str">
+        <f>VLOOKUP(A63,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63" s="9">
+        <v>318</v>
+      </c>
+      <c r="E63" s="9">
+        <v>21214213</v>
+      </c>
+      <c r="F63" s="9">
+        <v>3021298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>12</v>
+      </c>
+      <c r="B64" t="str">
+        <f>VLOOKUP(A64,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64" s="9">
+        <v>317</v>
+      </c>
+      <c r="E64" s="9">
+        <v>54000202</v>
+      </c>
+      <c r="F64" s="9">
+        <v>9190695</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65">
+        <v>13</v>
+      </c>
+      <c r="B65" t="str">
+        <f>VLOOKUP(A65,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" s="9">
+        <v>488</v>
+      </c>
+      <c r="E65" s="9">
+        <v>2598918</v>
+      </c>
+      <c r="F65" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66">
+        <v>13</v>
+      </c>
+      <c r="B66" t="str">
+        <f>VLOOKUP(A66,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66" s="9">
+        <v>488</v>
+      </c>
+      <c r="E66" s="9">
+        <v>11237579</v>
+      </c>
+      <c r="F66" s="9">
+        <v>393258</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67">
+        <v>13</v>
+      </c>
+      <c r="B67" t="str">
+        <f>VLOOKUP(A67,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67" s="9">
+        <v>487</v>
+      </c>
+      <c r="E67" s="9">
+        <v>19817269</v>
+      </c>
+      <c r="F67" s="9">
+        <v>1834009</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68">
+        <v>13</v>
+      </c>
+      <c r="B68" t="str">
+        <f>VLOOKUP(A68,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" s="9">
+        <v>488</v>
+      </c>
+      <c r="E68" s="9">
+        <v>29303616</v>
+      </c>
+      <c r="F68" s="9">
+        <v>3659633</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69">
+        <v>13</v>
+      </c>
+      <c r="B69" t="str">
+        <f>VLOOKUP(A69,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69" s="9">
+        <v>487</v>
+      </c>
+      <c r="E69" s="9">
+        <v>58216199</v>
+      </c>
+      <c r="F69" s="9">
+        <v>9051372</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A70">
+        <v>14</v>
+      </c>
+      <c r="B70" t="str">
+        <f>VLOOKUP(A70,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" s="9">
+        <v>691</v>
+      </c>
+      <c r="E70" s="9">
+        <v>6072809</v>
+      </c>
+      <c r="F70" s="9">
+        <v>24484</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A71">
+        <v>14</v>
+      </c>
+      <c r="B71" t="str">
+        <f>VLOOKUP(A71,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71" s="9">
+        <v>691</v>
+      </c>
+      <c r="E71" s="9">
+        <v>23794968</v>
+      </c>
+      <c r="F71" s="9">
+        <v>1972651</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72">
+        <v>14</v>
+      </c>
+      <c r="B72" t="str">
+        <f>VLOOKUP(A72,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" s="9">
+        <v>691</v>
+      </c>
+      <c r="E72" s="9">
+        <v>37722820</v>
+      </c>
+      <c r="F72" s="9">
+        <v>4743479</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73">
+        <v>14</v>
+      </c>
+      <c r="B73" t="str">
+        <f>VLOOKUP(A73,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73" s="9">
+        <v>691</v>
+      </c>
+      <c r="E73" s="9">
+        <v>54527912</v>
+      </c>
+      <c r="F73" s="9">
+        <v>7858972</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74">
+        <v>14</v>
+      </c>
+      <c r="B74" t="str">
+        <f>VLOOKUP(A74,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74" s="9">
+        <v>691</v>
+      </c>
+      <c r="E74" s="9">
+        <v>131817656</v>
+      </c>
+      <c r="F74" s="9">
+        <v>22616293</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75">
+        <v>15</v>
+      </c>
+      <c r="B75" t="str">
+        <f>VLOOKUP(A75,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" s="9">
+        <v>1058</v>
+      </c>
+      <c r="E75" s="9">
+        <v>9321468</v>
+      </c>
+      <c r="F75" s="9">
+        <v>32877</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76">
+        <v>15</v>
+      </c>
+      <c r="B76" t="str">
+        <f>VLOOKUP(A76,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76" s="9">
+        <v>1058</v>
+      </c>
+      <c r="E76" s="9">
+        <v>35495823</v>
+      </c>
+      <c r="F76" s="9">
+        <v>2618620</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77">
+        <v>15</v>
+      </c>
+      <c r="B77" t="str">
+        <f>VLOOKUP(A77,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" s="9">
+        <v>1058</v>
+      </c>
+      <c r="E77" s="9">
+        <v>54340421</v>
+      </c>
+      <c r="F77" s="9">
+        <v>6052843</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>15</v>
+      </c>
+      <c r="B78" t="str">
+        <f>VLOOKUP(A78,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C78">
+        <v>4</v>
+      </c>
+      <c r="D78" s="9">
+        <v>1058</v>
+      </c>
+      <c r="E78" s="9">
+        <v>75595961</v>
+      </c>
+      <c r="F78" s="9">
+        <v>9529943</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A79">
+        <v>15</v>
+      </c>
+      <c r="B79" t="str">
+        <f>VLOOKUP(A79,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79" s="9">
+        <v>1057</v>
+      </c>
+      <c r="E79" s="9">
+        <v>139288169</v>
+      </c>
+      <c r="F79" s="9">
+        <v>21580220</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>16</v>
+      </c>
+      <c r="B80" t="str">
+        <f>VLOOKUP(A80,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" s="9">
+        <v>632</v>
+      </c>
+      <c r="E80" s="9">
+        <v>2873804</v>
+      </c>
+      <c r="F80" s="9">
+        <v>21249</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81">
+        <v>16</v>
+      </c>
+      <c r="B81" t="str">
+        <f>VLOOKUP(A81,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81" s="9">
+        <v>632</v>
+      </c>
+      <c r="E81" s="9">
+        <v>15137189</v>
+      </c>
+      <c r="F81" s="9">
+        <v>583802</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82">
+        <v>16</v>
+      </c>
+      <c r="B82" t="str">
+        <f>VLOOKUP(A82,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82" s="9">
+        <v>631</v>
+      </c>
+      <c r="E82" s="9">
+        <v>27072300</v>
+      </c>
+      <c r="F82" s="9">
+        <v>2643853</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83">
+        <v>16</v>
+      </c>
+      <c r="B83" t="str">
+        <f>VLOOKUP(A83,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="D83" s="9">
+        <v>632</v>
+      </c>
+      <c r="E83" s="9">
+        <v>38895220</v>
+      </c>
+      <c r="F83" s="9">
+        <v>4702754</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A84">
+        <v>16</v>
+      </c>
+      <c r="B84" t="str">
+        <f>VLOOKUP(A84,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+      <c r="D84" s="9">
+        <v>631</v>
+      </c>
+      <c r="E84" s="9">
+        <v>79568347</v>
+      </c>
+      <c r="F84" s="9">
+        <v>12263342</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A85">
+        <v>17</v>
+      </c>
+      <c r="B85" t="str">
+        <f>VLOOKUP(A85,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" s="9">
+        <v>1811</v>
+      </c>
+      <c r="E85" s="9">
+        <v>6519988</v>
+      </c>
+      <c r="F85" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A86">
+        <v>17</v>
+      </c>
+      <c r="B86" t="str">
+        <f>VLOOKUP(A86,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" s="9">
+        <v>1810</v>
+      </c>
+      <c r="E86" s="9">
+        <v>36861499</v>
+      </c>
+      <c r="F86" s="9">
+        <v>799087</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A87">
+        <v>17</v>
+      </c>
+      <c r="B87" t="str">
+        <f>VLOOKUP(A87,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" s="9">
+        <v>1811</v>
+      </c>
+      <c r="E87" s="9">
+        <v>69525408</v>
+      </c>
+      <c r="F87" s="9">
+        <v>6051723</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A88">
+        <v>17</v>
+      </c>
+      <c r="B88" t="str">
+        <f>VLOOKUP(A88,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="D88" s="9">
+        <v>1810</v>
+      </c>
+      <c r="E88" s="9">
+        <v>105865677</v>
+      </c>
+      <c r="F88" s="9">
+        <v>12729152</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89">
+        <v>17</v>
+      </c>
+      <c r="B89" t="str">
+        <f>VLOOKUP(A89,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C89">
+        <v>5</v>
+      </c>
+      <c r="D89" s="9">
+        <v>1810</v>
+      </c>
+      <c r="E89" s="9">
+        <v>234225737</v>
+      </c>
+      <c r="F89" s="9">
+        <v>37568246</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90">
+        <v>18</v>
+      </c>
+      <c r="B90" t="str">
+        <f>VLOOKUP(A90,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90" s="9">
+        <v>819</v>
+      </c>
+      <c r="E90" s="9">
+        <v>3257396</v>
+      </c>
+      <c r="F90" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91">
+        <v>18</v>
+      </c>
+      <c r="B91" t="str">
+        <f>VLOOKUP(A91,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" s="9">
+        <v>819</v>
+      </c>
+      <c r="E91" s="9">
+        <v>17101729</v>
+      </c>
+      <c r="F91" s="9">
+        <v>382611</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92">
+        <v>18</v>
+      </c>
+      <c r="B92" t="str">
+        <f>VLOOKUP(A92,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+      <c r="D92" s="9">
+        <v>818</v>
+      </c>
+      <c r="E92" s="9">
+        <v>30508976</v>
+      </c>
+      <c r="F92" s="9">
+        <v>2550599</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A93">
+        <v>18</v>
+      </c>
+      <c r="B93" t="str">
+        <f>VLOOKUP(A93,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C93">
+        <v>4</v>
+      </c>
+      <c r="D93" s="9">
+        <v>819</v>
+      </c>
+      <c r="E93" s="9">
+        <v>44272287</v>
+      </c>
+      <c r="F93" s="9">
+        <v>4555972</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A94">
+        <v>18</v>
+      </c>
+      <c r="B94" t="str">
+        <f>VLOOKUP(A94,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
+      </c>
+      <c r="D94" s="9">
+        <v>818</v>
+      </c>
+      <c r="E94" s="9">
+        <v>77917765</v>
+      </c>
+      <c r="F94" s="9">
+        <v>10773948</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A95">
+        <v>19</v>
+      </c>
+      <c r="B95" t="str">
+        <f>VLOOKUP(A95,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95" s="9">
+        <v>322</v>
+      </c>
+      <c r="E95" s="9">
+        <v>1589281</v>
+      </c>
+      <c r="F95" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A96">
+        <v>19</v>
+      </c>
+      <c r="B96" t="str">
+        <f>VLOOKUP(A96,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96" s="9">
+        <v>322</v>
+      </c>
+      <c r="E96" s="9">
+        <v>7757056</v>
+      </c>
+      <c r="F96" s="9">
+        <v>263755</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A97">
+        <v>19</v>
+      </c>
+      <c r="B97" t="str">
+        <f>VLOOKUP(A97,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97" s="9">
+        <v>323</v>
+      </c>
+      <c r="E97" s="9">
+        <v>13393286</v>
+      </c>
+      <c r="F97" s="9">
+        <v>1145092</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A98">
+        <v>19</v>
+      </c>
+      <c r="B98" t="str">
+        <f>VLOOKUP(A98,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98" s="9">
+        <v>321</v>
+      </c>
+      <c r="E98" s="9">
+        <v>18877774</v>
+      </c>
+      <c r="F98" s="9">
+        <v>1998744</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A99">
+        <v>19</v>
+      </c>
+      <c r="B99" t="str">
+        <f>VLOOKUP(A99,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C99">
+        <v>5</v>
+      </c>
+      <c r="D99" s="9">
+        <v>321</v>
+      </c>
+      <c r="E99" s="9">
+        <v>32323431</v>
+      </c>
+      <c r="F99" s="9">
+        <v>4490346</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A100">
+        <v>20</v>
+      </c>
+      <c r="B100" t="str">
+        <f>VLOOKUP(A100,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100" s="9">
+        <v>2352</v>
+      </c>
+      <c r="E100" s="9">
+        <v>20301802</v>
+      </c>
+      <c r="F100" s="9">
+        <v>171673</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A101">
+        <v>20</v>
+      </c>
+      <c r="B101" t="str">
+        <f>VLOOKUP(A101,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" s="9">
+        <v>2352</v>
+      </c>
+      <c r="E101" s="9">
+        <v>89283464</v>
+      </c>
+      <c r="F101" s="9">
+        <v>7420987</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A102">
+        <v>20</v>
+      </c>
+      <c r="B102" t="str">
+        <f>VLOOKUP(A102,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
+      </c>
+      <c r="D102" s="9">
+        <v>2351</v>
+      </c>
+      <c r="E102" s="9">
+        <v>149676110</v>
+      </c>
+      <c r="F102" s="9">
+        <v>17880919</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A103">
+        <v>20</v>
+      </c>
+      <c r="B103" t="str">
+        <f>VLOOKUP(A103,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103" s="9">
+        <v>2352</v>
+      </c>
+      <c r="E103" s="9">
+        <v>226731684</v>
+      </c>
+      <c r="F103" s="9">
+        <v>30918010</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A104">
+        <v>20</v>
+      </c>
+      <c r="B104" t="str">
+        <f>VLOOKUP(A104,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C104">
+        <v>5</v>
+      </c>
+      <c r="D104" s="9">
+        <v>2351</v>
+      </c>
+      <c r="E104" s="9">
+        <v>582402265</v>
+      </c>
+      <c r="F104" s="9">
+        <v>101504376</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A105">
+        <v>30</v>
+      </c>
+      <c r="B105" t="str">
+        <f>VLOOKUP(A105,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" s="9">
+        <v>126</v>
+      </c>
+      <c r="E105" s="9">
+        <v>881961</v>
+      </c>
+      <c r="F105" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A106">
+        <v>30</v>
+      </c>
+      <c r="B106" t="str">
+        <f>VLOOKUP(A106,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106" s="9">
+        <v>126</v>
+      </c>
+      <c r="E106" s="9">
+        <v>4514929</v>
+      </c>
+      <c r="F106" s="9">
+        <v>324794</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A107">
+        <v>30</v>
+      </c>
+      <c r="B107" t="str">
+        <f>VLOOKUP(A107,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
+      </c>
+      <c r="D107" s="9">
+        <v>125</v>
+      </c>
+      <c r="E107" s="9">
+        <v>8631876</v>
+      </c>
+      <c r="F107" s="9">
+        <v>1019910</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A108">
+        <v>30</v>
+      </c>
+      <c r="B108" t="str">
+        <f>VLOOKUP(A108,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C108">
+        <v>4</v>
+      </c>
+      <c r="D108" s="9">
+        <v>126</v>
+      </c>
+      <c r="E108" s="9">
+        <v>14162521</v>
+      </c>
+      <c r="F108" s="9">
+        <v>1904172</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A109">
+        <v>30</v>
+      </c>
+      <c r="B109" t="str">
+        <f>VLOOKUP(A109,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C109">
+        <v>5</v>
+      </c>
+      <c r="D109" s="9">
+        <v>125</v>
+      </c>
+      <c r="E109" s="9">
+        <v>48624742</v>
+      </c>
+      <c r="F109" s="9">
+        <v>8974933</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="C111" t="s">
+        <v>20</v>
+      </c>
+      <c r="D111" s="2">
+        <f>SUM(D5:D109)</f>
+        <v>115380</v>
+      </c>
+      <c r="E111" s="2">
+        <f>SUM(E5:E109)</f>
+        <v>7874426113</v>
+      </c>
+      <c r="F111" s="2">
+        <f>SUM(F5:F109)</f>
+        <v>1115105002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView topLeftCell="A92" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G111" sqref="D111:G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6042,8 +8333,2283 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94E1ACB-C1A3-994E-AE99-9A35AAA9A062}">
+  <dimension ref="A1:F111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>335</v>
+      </c>
+      <c r="E5" s="9">
+        <v>127668</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9">
+        <v>335</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2840991</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9">
+        <v>335</v>
+      </c>
+      <c r="E7" s="9">
+        <v>11839779</v>
+      </c>
+      <c r="F7" s="9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9">
+        <v>335</v>
+      </c>
+      <c r="E8" s="9">
+        <v>58489345</v>
+      </c>
+      <c r="F8" s="9">
+        <v>104183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="str">
+        <f>VLOOKUP(A9,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Grossbasel</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="9">
+        <v>335</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1627102950</v>
+      </c>
+      <c r="F9" s="9">
+        <v>9132731</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="str">
+        <f>VLOOKUP(A10,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>600</v>
+      </c>
+      <c r="E10" s="9">
+        <v>32190</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="str">
+        <f>VLOOKUP(A11,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9">
+        <v>600</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4344744</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="str">
+        <f>VLOOKUP(A12,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="9">
+        <v>600</v>
+      </c>
+      <c r="E12" s="9">
+        <v>28634139</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="str">
+        <f>VLOOKUP(A13,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
+        <v>600</v>
+      </c>
+      <c r="E13" s="9">
+        <v>131116864</v>
+      </c>
+      <c r="F13" s="9">
+        <v>268160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="str">
+        <f>VLOOKUP(A14,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Vorstaedte</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9">
+        <v>599</v>
+      </c>
+      <c r="E14" s="9">
+        <v>4012478672</v>
+      </c>
+      <c r="F14" s="9">
+        <v>18221629</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="str">
+        <f>VLOOKUP(A15,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1248</v>
+      </c>
+      <c r="E15" s="9">
+        <v>25604</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1248</v>
+      </c>
+      <c r="E16" s="9">
+        <v>7156042</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="str">
+        <f>VLOOKUP(A17,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1248</v>
+      </c>
+      <c r="E17" s="9">
+        <v>48426539</v>
+      </c>
+      <c r="F17" s="9">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="str">
+        <f>VLOOKUP(A18,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1248</v>
+      </c>
+      <c r="E18" s="9">
+        <v>221771547</v>
+      </c>
+      <c r="F18" s="9">
+        <v>370114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP(A19,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Am Ring</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1247</v>
+      </c>
+      <c r="E19" s="9">
+        <v>2439182375</v>
+      </c>
+      <c r="F19" s="9">
+        <v>12487875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1201</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP(A21,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="9">
+        <v>998</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1816111</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="str">
+        <f>VLOOKUP(A22,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1100</v>
+      </c>
+      <c r="E22" s="9">
+        <v>16274476</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="str">
+        <f>VLOOKUP(A23,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1099</v>
+      </c>
+      <c r="E23" s="9">
+        <v>74524282</v>
+      </c>
+      <c r="F23" s="9">
+        <v>20675</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="str">
+        <f>VLOOKUP(A24,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Breite</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24" s="9">
+        <v>1099</v>
+      </c>
+      <c r="E24" s="9">
+        <v>677846059</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2798970</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="str">
+        <f>VLOOKUP(A25,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1288</v>
+      </c>
+      <c r="E25" s="9">
+        <v>91217</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="str">
+        <f>VLOOKUP(A26,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1288</v>
+      </c>
+      <c r="E26" s="9">
+        <v>12171579</v>
+      </c>
+      <c r="F26" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="str">
+        <f>VLOOKUP(A27,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1288</v>
+      </c>
+      <c r="E27" s="9">
+        <v>77977103</v>
+      </c>
+      <c r="F27" s="9">
+        <v>15978</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="str">
+        <f>VLOOKUP(A28,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1288</v>
+      </c>
+      <c r="E28" s="9">
+        <v>330709194</v>
+      </c>
+      <c r="F28" s="9">
+        <v>757059</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" t="str">
+        <f>VLOOKUP(A29,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Alban</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1287</v>
+      </c>
+      <c r="E29" s="9">
+        <v>6235667749</v>
+      </c>
+      <c r="F29" s="9">
+        <v>36467745</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="str">
+        <f>VLOOKUP(A30,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="9">
+        <v>2723</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="str">
+        <f>VLOOKUP(A31,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="9">
+        <v>1894</v>
+      </c>
+      <c r="E31" s="9">
+        <v>2583751</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="str">
+        <f>VLOOKUP(A32,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" s="9">
+        <v>2308</v>
+      </c>
+      <c r="E32" s="9">
+        <v>28566290</v>
+      </c>
+      <c r="F32" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="str">
+        <f>VLOOKUP(A33,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" s="9">
+        <v>2308</v>
+      </c>
+      <c r="E33" s="9">
+        <v>134756699</v>
+      </c>
+      <c r="F33" s="9">
+        <v>25993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="str">
+        <f>VLOOKUP(A34,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gundeldingen</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34" s="9">
+        <v>2308</v>
+      </c>
+      <c r="E34" s="9">
+        <v>1511531962</v>
+      </c>
+      <c r="F34" s="9">
+        <v>6353278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" t="str">
+        <f>VLOOKUP(A35,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1004</v>
+      </c>
+      <c r="E35" s="9">
+        <v>70098</v>
+      </c>
+      <c r="F35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36" t="str">
+        <f>VLOOKUP(A36,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="9">
+        <v>991</v>
+      </c>
+      <c r="E36" s="9">
+        <v>10188488</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37" t="str">
+        <f>VLOOKUP(A37,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" s="9">
+        <v>997</v>
+      </c>
+      <c r="E37" s="9">
+        <v>69200973</v>
+      </c>
+      <c r="F37" s="9">
+        <v>22069</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="str">
+        <f>VLOOKUP(A38,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" s="9">
+        <v>997</v>
+      </c>
+      <c r="E38" s="9">
+        <v>312416913</v>
+      </c>
+      <c r="F38" s="9">
+        <v>803083</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" t="str">
+        <f>VLOOKUP(A39,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bruderholz</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39" s="9">
+        <v>997</v>
+      </c>
+      <c r="E39" s="9">
+        <v>12169879848</v>
+      </c>
+      <c r="F39" s="9">
+        <v>89278854</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40" t="str">
+        <f>VLOOKUP(A40,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9">
+        <v>1623</v>
+      </c>
+      <c r="E40" s="9">
+        <v>13425</v>
+      </c>
+      <c r="F40" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="B41" t="str">
+        <f>VLOOKUP(A41,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="9">
+        <v>1622</v>
+      </c>
+      <c r="E41" s="9">
+        <v>10159710</v>
+      </c>
+      <c r="F41" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42" t="str">
+        <f>VLOOKUP(A42,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" s="9">
+        <v>1623</v>
+      </c>
+      <c r="E42" s="9">
+        <v>64340564</v>
+      </c>
+      <c r="F42" s="9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43" t="str">
+        <f>VLOOKUP(A43,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43" s="9">
+        <v>1622</v>
+      </c>
+      <c r="E43" s="9">
+        <v>295728960</v>
+      </c>
+      <c r="F43" s="9">
+        <v>495230</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="str">
+        <f>VLOOKUP(A44,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bachletten</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44" s="9">
+        <v>1622</v>
+      </c>
+      <c r="E44" s="9">
+        <v>2984583063</v>
+      </c>
+      <c r="F44" s="9">
+        <v>14735916</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="str">
+        <f>VLOOKUP(A45,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="9">
+        <v>840</v>
+      </c>
+      <c r="E45" s="9">
+        <v>9560</v>
+      </c>
+      <c r="F45" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46" t="str">
+        <f>VLOOKUP(A46,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="9">
+        <v>837</v>
+      </c>
+      <c r="E46" s="9">
+        <v>3747635</v>
+      </c>
+      <c r="F46" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47" t="str">
+        <f>VLOOKUP(A47,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" s="9">
+        <v>838</v>
+      </c>
+      <c r="E47" s="9">
+        <v>25370995</v>
+      </c>
+      <c r="F47" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="B48" t="str">
+        <f>VLOOKUP(A48,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" s="9">
+        <v>838</v>
+      </c>
+      <c r="E48" s="9">
+        <v>106572209</v>
+      </c>
+      <c r="F48" s="9">
+        <v>122274</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49" t="str">
+        <f>VLOOKUP(A49,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Gotthelf</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49" s="9">
+        <v>838</v>
+      </c>
+      <c r="E49" s="9">
+        <v>828072431</v>
+      </c>
+      <c r="F49" s="9">
+        <v>3911098</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50" t="str">
+        <f>VLOOKUP(A50,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" s="9">
+        <v>2456</v>
+      </c>
+      <c r="E50" s="9">
+        <v>0</v>
+      </c>
+      <c r="F50" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51" t="str">
+        <f>VLOOKUP(A51,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" s="9">
+        <v>1440</v>
+      </c>
+      <c r="E51" s="9">
+        <v>1445050</v>
+      </c>
+      <c r="F51" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52" t="str">
+        <f>VLOOKUP(A52,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" s="9">
+        <v>1948</v>
+      </c>
+      <c r="E52" s="9">
+        <v>19344628</v>
+      </c>
+      <c r="F52" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53" t="str">
+        <f>VLOOKUP(A53,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53" s="9">
+        <v>1948</v>
+      </c>
+      <c r="E53" s="9">
+        <v>106608248</v>
+      </c>
+      <c r="F53" s="9">
+        <v>18437</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54" t="str">
+        <f>VLOOKUP(A54,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Iselin</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54" s="9">
+        <v>1947</v>
+      </c>
+      <c r="E54" s="9">
+        <v>1139769915</v>
+      </c>
+      <c r="F54" s="9">
+        <v>4346933</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>11</v>
+      </c>
+      <c r="B55" t="str">
+        <f>VLOOKUP(A55,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" s="9">
+        <v>2917</v>
+      </c>
+      <c r="E55" s="9">
+        <v>0</v>
+      </c>
+      <c r="F55" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>11</v>
+      </c>
+      <c r="B56" t="str">
+        <f>VLOOKUP(A56,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" s="9">
+        <v>1441</v>
+      </c>
+      <c r="E56" s="9">
+        <v>1095203</v>
+      </c>
+      <c r="F56" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>11</v>
+      </c>
+      <c r="B57" t="str">
+        <f>VLOOKUP(A57,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" s="9">
+        <v>2179</v>
+      </c>
+      <c r="E57" s="9">
+        <v>17335340</v>
+      </c>
+      <c r="F57" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>11</v>
+      </c>
+      <c r="B58" t="str">
+        <f>VLOOKUP(A58,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" s="9">
+        <v>2179</v>
+      </c>
+      <c r="E58" s="9">
+        <v>104015671</v>
+      </c>
+      <c r="F58" s="9">
+        <v>9739</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>11</v>
+      </c>
+      <c r="B59" t="str">
+        <f>VLOOKUP(A59,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>St. Johann</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59" s="9">
+        <v>2178</v>
+      </c>
+      <c r="E59" s="9">
+        <v>1314938933</v>
+      </c>
+      <c r="F59" s="9">
+        <v>5545306</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60">
+        <v>12</v>
+      </c>
+      <c r="B60" t="str">
+        <f>VLOOKUP(A60,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" s="9">
+        <v>412</v>
+      </c>
+      <c r="E60" s="9">
+        <v>0</v>
+      </c>
+      <c r="F60" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61">
+        <v>12</v>
+      </c>
+      <c r="B61" t="str">
+        <f>VLOOKUP(A61,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" s="9">
+        <v>224</v>
+      </c>
+      <c r="E61" s="9">
+        <v>234101</v>
+      </c>
+      <c r="F61" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>12</v>
+      </c>
+      <c r="B62" t="str">
+        <f>VLOOKUP(A62,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" s="9">
+        <v>317</v>
+      </c>
+      <c r="E62" s="9">
+        <v>3154802</v>
+      </c>
+      <c r="F62" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>12</v>
+      </c>
+      <c r="B63" t="str">
+        <f>VLOOKUP(A63,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63" s="9">
+        <v>318</v>
+      </c>
+      <c r="E63" s="9">
+        <v>18233888</v>
+      </c>
+      <c r="F63" s="9">
+        <v>4037</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>12</v>
+      </c>
+      <c r="B64" t="str">
+        <f>VLOOKUP(A64,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Altstadt Kleinbasel</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64" s="9">
+        <v>317</v>
+      </c>
+      <c r="E64" s="9">
+        <v>373911233</v>
+      </c>
+      <c r="F64" s="9">
+        <v>1780144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65">
+        <v>13</v>
+      </c>
+      <c r="B65" t="str">
+        <f>VLOOKUP(A65,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" s="9">
+        <v>617</v>
+      </c>
+      <c r="E65" s="9">
+        <v>0</v>
+      </c>
+      <c r="F65" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66">
+        <v>13</v>
+      </c>
+      <c r="B66" t="str">
+        <f>VLOOKUP(A66,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66" s="9">
+        <v>359</v>
+      </c>
+      <c r="E66" s="9">
+        <v>339395</v>
+      </c>
+      <c r="F66" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67">
+        <v>13</v>
+      </c>
+      <c r="B67" t="str">
+        <f>VLOOKUP(A67,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67" s="9">
+        <v>487</v>
+      </c>
+      <c r="E67" s="9">
+        <v>4436285</v>
+      </c>
+      <c r="F67" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68">
+        <v>13</v>
+      </c>
+      <c r="B68" t="str">
+        <f>VLOOKUP(A68,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" s="9">
+        <v>488</v>
+      </c>
+      <c r="E68" s="9">
+        <v>22237805</v>
+      </c>
+      <c r="F68" s="9">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69">
+        <v>13</v>
+      </c>
+      <c r="B69" t="str">
+        <f>VLOOKUP(A69,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Clara</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69" s="9">
+        <v>487</v>
+      </c>
+      <c r="E69" s="9">
+        <v>290326328</v>
+      </c>
+      <c r="F69" s="9">
+        <v>1237522</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A70">
+        <v>14</v>
+      </c>
+      <c r="B70" t="str">
+        <f>VLOOKUP(A70,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" s="9">
+        <v>691</v>
+      </c>
+      <c r="E70" s="9">
+        <v>2978</v>
+      </c>
+      <c r="F70" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A71">
+        <v>14</v>
+      </c>
+      <c r="B71" t="str">
+        <f>VLOOKUP(A71,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71" s="9">
+        <v>691</v>
+      </c>
+      <c r="E71" s="9">
+        <v>3004135</v>
+      </c>
+      <c r="F71" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72">
+        <v>14</v>
+      </c>
+      <c r="B72" t="str">
+        <f>VLOOKUP(A72,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" s="9">
+        <v>691</v>
+      </c>
+      <c r="E72" s="9">
+        <v>20821284</v>
+      </c>
+      <c r="F72" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73">
+        <v>14</v>
+      </c>
+      <c r="B73" t="str">
+        <f>VLOOKUP(A73,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73" s="9">
+        <v>691</v>
+      </c>
+      <c r="E73" s="9">
+        <v>91803573</v>
+      </c>
+      <c r="F73" s="9">
+        <v>109779</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74">
+        <v>14</v>
+      </c>
+      <c r="B74" t="str">
+        <f>VLOOKUP(A74,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Wettstein</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74" s="9">
+        <v>691</v>
+      </c>
+      <c r="E74" s="9">
+        <v>907124743</v>
+      </c>
+      <c r="F74" s="9">
+        <v>4481771</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75">
+        <v>15</v>
+      </c>
+      <c r="B75" t="str">
+        <f>VLOOKUP(A75,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" s="9">
+        <v>1165</v>
+      </c>
+      <c r="E75" s="9">
+        <v>0</v>
+      </c>
+      <c r="F75" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76">
+        <v>15</v>
+      </c>
+      <c r="B76" t="str">
+        <f>VLOOKUP(A76,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76" s="9">
+        <v>951</v>
+      </c>
+      <c r="E76" s="9">
+        <v>2100405</v>
+      </c>
+      <c r="F76" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77">
+        <v>15</v>
+      </c>
+      <c r="B77" t="str">
+        <f>VLOOKUP(A77,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" s="9">
+        <v>1058</v>
+      </c>
+      <c r="E77" s="9">
+        <v>18601575</v>
+      </c>
+      <c r="F77" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>15</v>
+      </c>
+      <c r="B78" t="str">
+        <f>VLOOKUP(A78,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C78">
+        <v>4</v>
+      </c>
+      <c r="D78" s="9">
+        <v>1058</v>
+      </c>
+      <c r="E78" s="9">
+        <v>90717977</v>
+      </c>
+      <c r="F78" s="9">
+        <v>41074</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A79">
+        <v>15</v>
+      </c>
+      <c r="B79" t="str">
+        <f>VLOOKUP(A79,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Hirzbrunnen</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79" s="9">
+        <v>1057</v>
+      </c>
+      <c r="E79" s="9">
+        <v>872713332</v>
+      </c>
+      <c r="F79" s="9">
+        <v>3849474</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>16</v>
+      </c>
+      <c r="B80" t="str">
+        <f>VLOOKUP(A80,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" s="9">
+        <v>1020</v>
+      </c>
+      <c r="E80" s="9">
+        <v>0</v>
+      </c>
+      <c r="F80" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81">
+        <v>16</v>
+      </c>
+      <c r="B81" t="str">
+        <f>VLOOKUP(A81,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81" s="9">
+        <v>244</v>
+      </c>
+      <c r="E81" s="9">
+        <v>64050</v>
+      </c>
+      <c r="F81" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82">
+        <v>16</v>
+      </c>
+      <c r="B82" t="str">
+        <f>VLOOKUP(A82,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82" s="9">
+        <v>631</v>
+      </c>
+      <c r="E82" s="9">
+        <v>2328227</v>
+      </c>
+      <c r="F82" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83">
+        <v>16</v>
+      </c>
+      <c r="B83" t="str">
+        <f>VLOOKUP(A83,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="D83" s="9">
+        <v>632</v>
+      </c>
+      <c r="E83" s="9">
+        <v>16071465</v>
+      </c>
+      <c r="F83" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A84">
+        <v>16</v>
+      </c>
+      <c r="B84" t="str">
+        <f>VLOOKUP(A84,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Rosental</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+      <c r="D84" s="9">
+        <v>631</v>
+      </c>
+      <c r="E84" s="9">
+        <v>224588797</v>
+      </c>
+      <c r="F84" s="9">
+        <v>802570</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A85">
+        <v>17</v>
+      </c>
+      <c r="B85" t="str">
+        <f>VLOOKUP(A85,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" s="9">
+        <v>2759</v>
+      </c>
+      <c r="E85" s="9">
+        <v>0</v>
+      </c>
+      <c r="F85" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A86">
+        <v>17</v>
+      </c>
+      <c r="B86" t="str">
+        <f>VLOOKUP(A86,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" s="9">
+        <v>892</v>
+      </c>
+      <c r="E86" s="9">
+        <v>328023</v>
+      </c>
+      <c r="F86" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A87">
+        <v>17</v>
+      </c>
+      <c r="B87" t="str">
+        <f>VLOOKUP(A87,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" s="9">
+        <v>1781</v>
+      </c>
+      <c r="E87" s="9">
+        <v>9583290</v>
+      </c>
+      <c r="F87" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A88">
+        <v>17</v>
+      </c>
+      <c r="B88" t="str">
+        <f>VLOOKUP(A88,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="D88" s="9">
+        <v>1810</v>
+      </c>
+      <c r="E88" s="9">
+        <v>69006576</v>
+      </c>
+      <c r="F88" s="9">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89">
+        <v>17</v>
+      </c>
+      <c r="B89" t="str">
+        <f>VLOOKUP(A89,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Matthaeus</v>
+      </c>
+      <c r="C89">
+        <v>5</v>
+      </c>
+      <c r="D89" s="9">
+        <v>1810</v>
+      </c>
+      <c r="E89" s="9">
+        <v>1085373033</v>
+      </c>
+      <c r="F89" s="9">
+        <v>4448137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90">
+        <v>18</v>
+      </c>
+      <c r="B90" t="str">
+        <f>VLOOKUP(A90,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90" s="9">
+        <v>1452</v>
+      </c>
+      <c r="E90" s="9">
+        <v>0</v>
+      </c>
+      <c r="F90" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91">
+        <v>18</v>
+      </c>
+      <c r="B91" t="str">
+        <f>VLOOKUP(A91,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" s="9">
+        <v>186</v>
+      </c>
+      <c r="E91" s="9">
+        <v>9562</v>
+      </c>
+      <c r="F91" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92">
+        <v>18</v>
+      </c>
+      <c r="B92" t="str">
+        <f>VLOOKUP(A92,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+      <c r="D92" s="9">
+        <v>818</v>
+      </c>
+      <c r="E92" s="9">
+        <v>1595694</v>
+      </c>
+      <c r="F92" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A93">
+        <v>18</v>
+      </c>
+      <c r="B93" t="str">
+        <f>VLOOKUP(A93,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C93">
+        <v>4</v>
+      </c>
+      <c r="D93" s="9">
+        <v>819</v>
+      </c>
+      <c r="E93" s="9">
+        <v>13924083</v>
+      </c>
+      <c r="F93" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A94">
+        <v>18</v>
+      </c>
+      <c r="B94" t="str">
+        <f>VLOOKUP(A94,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Klybeck</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
+      </c>
+      <c r="D94" s="9">
+        <v>818</v>
+      </c>
+      <c r="E94" s="9">
+        <v>226973065</v>
+      </c>
+      <c r="F94" s="9">
+        <v>760885</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A95">
+        <v>19</v>
+      </c>
+      <c r="B95" t="str">
+        <f>VLOOKUP(A95,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95" s="9">
+        <v>521</v>
+      </c>
+      <c r="E95" s="9">
+        <v>0</v>
+      </c>
+      <c r="F95" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A96">
+        <v>19</v>
+      </c>
+      <c r="B96" t="str">
+        <f>VLOOKUP(A96,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96" s="9">
+        <v>123</v>
+      </c>
+      <c r="E96" s="9">
+        <v>22622</v>
+      </c>
+      <c r="F96" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A97">
+        <v>19</v>
+      </c>
+      <c r="B97" t="str">
+        <f>VLOOKUP(A97,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+      <c r="D97" s="9">
+        <v>322</v>
+      </c>
+      <c r="E97" s="9">
+        <v>1069439</v>
+      </c>
+      <c r="F97" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A98">
+        <v>19</v>
+      </c>
+      <c r="B98" t="str">
+        <f>VLOOKUP(A98,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98" s="9">
+        <v>322</v>
+      </c>
+      <c r="E98" s="9">
+        <v>8611386</v>
+      </c>
+      <c r="F98" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A99">
+        <v>19</v>
+      </c>
+      <c r="B99" t="str">
+        <f>VLOOKUP(A99,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Kleinhueningen</v>
+      </c>
+      <c r="C99">
+        <v>5</v>
+      </c>
+      <c r="D99" s="9">
+        <v>321</v>
+      </c>
+      <c r="E99" s="9">
+        <v>100731848</v>
+      </c>
+      <c r="F99" s="9">
+        <v>332839</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A100">
+        <v>20</v>
+      </c>
+      <c r="B100" t="str">
+        <f>VLOOKUP(A100,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100" s="9">
+        <v>2352</v>
+      </c>
+      <c r="E100" s="9">
+        <v>78938</v>
+      </c>
+      <c r="F100" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A101">
+        <v>20</v>
+      </c>
+      <c r="B101" t="str">
+        <f>VLOOKUP(A101,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" s="9">
+        <v>2352</v>
+      </c>
+      <c r="E101" s="9">
+        <v>16679460</v>
+      </c>
+      <c r="F101" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A102">
+        <v>20</v>
+      </c>
+      <c r="B102" t="str">
+        <f>VLOOKUP(A102,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
+      </c>
+      <c r="D102" s="9">
+        <v>2351</v>
+      </c>
+      <c r="E102" s="9">
+        <v>122317052</v>
+      </c>
+      <c r="F102" s="9">
+        <v>13308</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A103">
+        <v>20</v>
+      </c>
+      <c r="B103" t="str">
+        <f>VLOOKUP(A103,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103" s="9">
+        <v>2352</v>
+      </c>
+      <c r="E103" s="9">
+        <v>597294056</v>
+      </c>
+      <c r="F103" s="9">
+        <v>1327597</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A104">
+        <v>20</v>
+      </c>
+      <c r="B104" t="str">
+        <f>VLOOKUP(A104,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Riehen</v>
+      </c>
+      <c r="C104">
+        <v>5</v>
+      </c>
+      <c r="D104" s="9">
+        <v>2351</v>
+      </c>
+      <c r="E104" s="9">
+        <v>6820552921</v>
+      </c>
+      <c r="F104" s="9">
+        <v>34825649</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A105">
+        <v>30</v>
+      </c>
+      <c r="B105" t="str">
+        <f>VLOOKUP(A105,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" s="9">
+        <v>126</v>
+      </c>
+      <c r="E105" s="9">
+        <v>16237</v>
+      </c>
+      <c r="F105" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A106">
+        <v>30</v>
+      </c>
+      <c r="B106" t="str">
+        <f>VLOOKUP(A106,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106" s="9">
+        <v>126</v>
+      </c>
+      <c r="E106" s="9">
+        <v>1234094</v>
+      </c>
+      <c r="F106" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A107">
+        <v>30</v>
+      </c>
+      <c r="B107" t="str">
+        <f>VLOOKUP(A107,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
+      </c>
+      <c r="D107" s="9">
+        <v>125</v>
+      </c>
+      <c r="E107" s="9">
+        <v>10834640</v>
+      </c>
+      <c r="F107" s="9">
+        <v>6090</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A108">
+        <v>30</v>
+      </c>
+      <c r="B108" t="str">
+        <f>VLOOKUP(A108,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C108">
+        <v>4</v>
+      </c>
+      <c r="D108" s="9">
+        <v>126</v>
+      </c>
+      <c r="E108" s="9">
+        <v>51162687</v>
+      </c>
+      <c r="F108" s="9">
+        <v>149605</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A109">
+        <v>30</v>
+      </c>
+      <c r="B109" t="str">
+        <f>VLOOKUP(A109,mapping_wohnviertel_id!$A$4:$B$24, 2)</f>
+        <v>Bettingen</v>
+      </c>
+      <c r="C109">
+        <v>5</v>
+      </c>
+      <c r="D109" s="9">
+        <v>125</v>
+      </c>
+      <c r="E109" s="9">
+        <v>1418790612</v>
+      </c>
+      <c r="F109" s="9">
+        <v>9597244</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="C111" t="s">
+        <v>20</v>
+      </c>
+      <c r="D111" s="2">
+        <f>SUM(D5:D109)</f>
+        <v>115380</v>
+      </c>
+      <c r="E111" s="2">
+        <f>SUM(E5:E109)</f>
+        <v>50801999477</v>
+      </c>
+      <c r="F111" s="2">
+        <f>SUM(F5:F109)</f>
+        <v>270086215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
@@ -6329,8 +10895,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -6530,8 +11096,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
@@ -6638,8 +11204,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">

</xml_diff>

<commit_message>
* Updated 2015 taxation data with correct GINI numbers * Added code to read GINI data
</commit_message>
<xml_diff>
--- a/data/Steuern_Klassen_Wohnviertel_cleaned.xlsx
+++ b/data/Steuern_Klassen_Wohnviertel_cleaned.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylan/Development/TaxationInequality_GIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13A0E1D9-8DE4-4C4A-8498-FC7049778809}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBDE8E7-8F2A-9D42-B805-D0635D3ABE84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="2" r:id="rId1"/>
-    <sheet name="Income_quintiles" sheetId="8" r:id="rId2"/>
-    <sheet name="Assets" sheetId="5" r:id="rId3"/>
-    <sheet name="Assets_quintiles" sheetId="9" r:id="rId4"/>
-    <sheet name="mapping_wohnviertel_geo_id" sheetId="7" r:id="rId5"/>
-    <sheet name="mapping_wohnviertel_id" sheetId="3" r:id="rId6"/>
-    <sheet name="mapping_incomeclass_id" sheetId="4" r:id="rId7"/>
-    <sheet name="mapping_assetclass_id" sheetId="6" r:id="rId8"/>
+    <sheet name="income_gini" sheetId="10" r:id="rId2"/>
+    <sheet name="Income_quintiles" sheetId="8" r:id="rId3"/>
+    <sheet name="Assets" sheetId="5" r:id="rId4"/>
+    <sheet name="assets_gini" sheetId="11" r:id="rId5"/>
+    <sheet name="Assets_quintiles" sheetId="9" r:id="rId6"/>
+    <sheet name="mapping_wohnviertel_geo_id" sheetId="7" r:id="rId7"/>
+    <sheet name="mapping_wohnviertel_id" sheetId="3" r:id="rId8"/>
+    <sheet name="mapping_incomeclass_id" sheetId="4" r:id="rId9"/>
+    <sheet name="mapping_assetclass_id" sheetId="6" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_AMO_SingleObject_151849305_ROM_F0.SEC2.Tabulate_1.SEC1.BDY.Kreuztabellenbericht_Tabelle_1" hidden="1">#REF!</definedName>
@@ -28,12 +30,12 @@
     <definedName name="_AMO_SingleObject_151849305_ROM_F0.SEC2.Tabulate_1.SEC1.HDR.TXT1" hidden="1">#REF!</definedName>
     <definedName name="_AMO_UniqueIdentifier" hidden="1">"'4ea23a4e-62ac-4326-a178-aa442716dc2f'"</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
   <si>
     <t>Altstadt Grossbasel</t>
   </si>
@@ -214,15 +216,22 @@
   <si>
     <t>assetquintile_id</t>
   </si>
+  <si>
+    <t>gini</t>
+  </si>
+  <si>
+    <t>wohnvirtel_id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -297,13 +306,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -313,13 +323,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard_t02.2.01" xfId="4" xr:uid="{0EB5F71F-2790-834C-BC02-955D1A1CC1C9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -658,7 +681,7 @@
   <dimension ref="A1:G233"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B109"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3358,7 +3381,386 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>49999</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>50000</v>
+      </c>
+      <c r="C5" s="7">
+        <v>99999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7">
+        <v>100000</v>
+      </c>
+      <c r="C6" s="7">
+        <v>299999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <v>300000</v>
+      </c>
+      <c r="C7" s="7">
+        <v>599999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7">
+        <v>700000</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1E+21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5250CF-8F9D-ED4A-B291-22E823B93F3A}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.63700000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.52100000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10">
+        <v>5</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.55800000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="10">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="10">
+        <v>8</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10">
+        <v>9</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.42799999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="10">
+        <v>11</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="10">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.53700000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="10">
+        <v>13</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="10">
+        <v>14</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.48699999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="10">
+        <v>15</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="10">
+        <v>16</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="10">
+        <v>17</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.503</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="10">
+        <v>18</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.435</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="10">
+        <v>19</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="10">
+        <v>20</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="10">
+        <v>30</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA76009E-9503-7840-9C54-03E7EF448422}">
   <dimension ref="A1:F111"/>
   <sheetViews>
@@ -5635,12 +6037,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G111" sqref="D111:G111"/>
+    <sheetView topLeftCell="A82" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8333,11 +8735,282 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3922145D-3645-6845-8B66-A062D36AF928}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.86499999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.84199999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10">
+        <v>5</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="10">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.95899999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="10">
+        <v>8</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0.85699999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10">
+        <v>9</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.85799999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="10">
+        <v>11</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="10">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="10">
+        <v>13</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.86499999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="10">
+        <v>14</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="10">
+        <v>15</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.84899999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="10">
+        <v>16</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="10">
+        <v>17</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="10">
+        <v>18</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="10">
+        <v>19</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.86399999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="10">
+        <v>20</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="10">
+        <v>30</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0.94799999999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94E1ACB-C1A3-994E-AE99-9A35AAA9A062}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -10608,7 +11281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -10895,7 +11568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -11096,7 +11769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -11202,113 +11875,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>49999</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7">
-        <v>50000</v>
-      </c>
-      <c r="C5" s="7">
-        <v>99999</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C6" s="7">
-        <v>299999</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" s="7">
-        <v>300000</v>
-      </c>
-      <c r="C7" s="7">
-        <v>599999</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7">
-        <v>700000</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1E+21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
* Updated data with marginal tax rates * Added expanded notebook
</commit_message>
<xml_diff>
--- a/data/Steuern_Klassen_Wohnviertel_cleaned.xlsx
+++ b/data/Steuern_Klassen_Wohnviertel_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylan/Development/TaxationInequality_GIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBDE8E7-8F2A-9D42-B805-D0635D3ABE84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41220A46-1FFD-2643-B598-031F06E1037D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28760" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
   <si>
     <t>Altstadt Grossbasel</t>
   </si>
@@ -222,6 +222,9 @@
   <si>
     <t>wohnvirtel_id</t>
   </si>
+  <si>
+    <t>marginal_tax_rate</t>
+  </si>
 </sst>
 </file>
 
@@ -306,14 +309,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -336,11 +340,15 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Standard_t02.2.01" xfId="4" xr:uid="{0EB5F71F-2790-834C-BC02-955D1A1CC1C9}"/>
   </cellStyles>
@@ -680,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G233"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -3495,7 +3503,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3762,10 +3770,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA76009E-9503-7840-9C54-03E7EF448422}">
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B109"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3779,18 +3787,18 @@
     <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -3809,8 +3817,11 @@
       <c r="F4" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G4" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3830,8 +3841,13 @@
       <c r="F5" s="9">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G5" s="15">
+        <f>F5/E5</f>
+        <v>1.5035106974786125E-4</v>
+      </c>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3851,8 +3867,13 @@
       <c r="F6" s="9">
         <v>184671</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G6" s="15">
+        <f t="shared" ref="G6:G69" si="0">F6/E6</f>
+        <v>2.6848798047740791E-2</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3872,8 +3893,13 @@
       <c r="F7" s="9">
         <v>2233910</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G7" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12845088375640937</v>
+      </c>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3893,8 +3919,13 @@
       <c r="F8" s="9">
         <v>5158796</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G8" s="15">
+        <f t="shared" si="0"/>
+        <v>0.16237343129464207</v>
+      </c>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3914,8 +3945,13 @@
       <c r="F9" s="9">
         <v>20323529</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G9" s="15">
+        <f t="shared" si="0"/>
+        <v>0.18998287141890488</v>
+      </c>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3935,8 +3971,12 @@
       <c r="F10" s="9">
         <v>11375</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G10" s="15">
+        <f t="shared" si="0"/>
+        <v>2.3114980925822552E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3956,8 +3996,12 @@
       <c r="F11" s="9">
         <v>1633999</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G11" s="15">
+        <f t="shared" si="0"/>
+        <v>8.1711062704527812E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3977,8 +4021,12 @@
       <c r="F12" s="9">
         <v>4822525</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G12" s="15">
+        <f t="shared" si="0"/>
+        <v>0.13586756321232021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3998,8 +4046,12 @@
       <c r="F13" s="9">
         <v>9116508</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G13" s="15">
+        <f t="shared" si="0"/>
+        <v>0.15741322393205887</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4019,8 +4071,12 @@
       <c r="F14" s="9">
         <v>33613224</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G14" s="15">
+        <f t="shared" si="0"/>
+        <v>0.18690570790814393</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>3</v>
       </c>
@@ -4040,8 +4096,12 @@
       <c r="F15" s="9">
         <v>5851</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G15" s="15">
+        <f t="shared" si="0"/>
+        <v>7.2174217780613813E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
@@ -4061,8 +4121,12 @@
       <c r="F16" s="9">
         <v>2465798</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G16" s="15">
+        <f t="shared" si="0"/>
+        <v>6.5632652113869261E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -4082,8 +4146,12 @@
       <c r="F17" s="9">
         <v>8228381</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G17" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12410843612768055</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
@@ -4103,8 +4171,12 @@
       <c r="F18" s="9">
         <v>15247132</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G18" s="15">
+        <f t="shared" si="0"/>
+        <v>0.14719125612540612</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3</v>
       </c>
@@ -4124,8 +4196,12 @@
       <c r="F19" s="9">
         <v>44649403</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G19" s="15">
+        <f t="shared" si="0"/>
+        <v>0.17332455827044016</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>4</v>
       </c>
@@ -4145,8 +4221,12 @@
       <c r="F20" s="9">
         <v>121398</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G20" s="15">
+        <f t="shared" si="0"/>
+        <v>1.1935606831880866E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>4</v>
       </c>
@@ -4166,8 +4246,12 @@
       <c r="F21" s="9">
         <v>2287363</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G21" s="15">
+        <f t="shared" si="0"/>
+        <v>6.668225157019507E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>4</v>
       </c>
@@ -4187,8 +4271,12 @@
       <c r="F22" s="9">
         <v>5838183</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G22" s="15">
+        <f t="shared" si="0"/>
+        <v>0.11124708821588987</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>4</v>
       </c>
@@ -4208,8 +4296,12 @@
       <c r="F23" s="9">
         <v>9258391</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G23" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12786634214276074</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>4</v>
       </c>
@@ -4229,8 +4321,12 @@
       <c r="F24" s="9">
         <v>22557320</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G24" s="15">
+        <f t="shared" si="0"/>
+        <v>0.16103184791693265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>5</v>
       </c>
@@ -4250,8 +4346,12 @@
       <c r="F25" s="9">
         <v>203057</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G25" s="15">
+        <f t="shared" si="0"/>
+        <v>1.4946755903930674E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>5</v>
       </c>
@@ -4271,8 +4371,12 @@
       <c r="F26" s="9">
         <v>4604127</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G26" s="15">
+        <f t="shared" si="0"/>
+        <v>9.1967852409331474E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>5</v>
       </c>
@@ -4292,8 +4396,12 @@
       <c r="F27" s="9">
         <v>10312084</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G27" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12996045022661795</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>5</v>
       </c>
@@ -4313,8 +4421,12 @@
       <c r="F28" s="9">
         <v>18460576</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G28" s="15">
+        <f t="shared" si="0"/>
+        <v>0.15112218803823832</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>5</v>
       </c>
@@ -4334,8 +4446,12 @@
       <c r="F29" s="9">
         <v>70654254</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G29" s="15">
+        <f t="shared" si="0"/>
+        <v>0.18506730269896984</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>6</v>
       </c>
@@ -4355,8 +4471,12 @@
       <c r="F30" s="9">
         <v>42477</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G30" s="15">
+        <f t="shared" si="0"/>
+        <v>2.5603038441807651E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>6</v>
       </c>
@@ -4376,8 +4496,12 @@
       <c r="F31" s="9">
         <v>3711308</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G31" s="15">
+        <f t="shared" si="0"/>
+        <v>5.6664140835423649E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>6</v>
       </c>
@@ -4397,8 +4521,12 @@
       <c r="F32" s="9">
         <v>12100789</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G32" s="15">
+        <f t="shared" si="0"/>
+        <v>0.11089616477516416</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>6</v>
       </c>
@@ -4418,8 +4546,12 @@
       <c r="F33" s="9">
         <v>20745338</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G33" s="15">
+        <f t="shared" si="0"/>
+        <v>0.13405703263851393</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>6</v>
       </c>
@@ -4439,8 +4571,12 @@
       <c r="F34" s="9">
         <v>46917663</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G34" s="15">
+        <f t="shared" si="0"/>
+        <v>0.15880886484369516</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>7</v>
       </c>
@@ -4460,8 +4596,12 @@
       <c r="F35" s="9">
         <v>34361</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G35" s="15">
+        <f t="shared" si="0"/>
+        <v>4.8107637005120737E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>7</v>
       </c>
@@ -4481,8 +4621,12 @@
       <c r="F36" s="9">
         <v>3212019</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G36" s="15">
+        <f t="shared" si="0"/>
+        <v>8.5862960958674073E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>7</v>
       </c>
@@ -4502,8 +4646,12 @@
       <c r="F37" s="9">
         <v>8384093</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G37" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12870379279606933</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>7</v>
       </c>
@@ -4523,8 +4671,12 @@
       <c r="F38" s="9">
         <v>15411942</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G38" s="15">
+        <f t="shared" si="0"/>
+        <v>0.14803034568193318</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>7</v>
       </c>
@@ -4544,8 +4696,12 @@
       <c r="F39" s="9">
         <v>71150407</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G39" s="15">
+        <f t="shared" si="0"/>
+        <v>0.19705584465607479</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>8</v>
       </c>
@@ -4565,8 +4721,12 @@
       <c r="F40" s="9">
         <v>104137</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G40" s="15">
+        <f>F40/E40</f>
+        <v>7.2072225454284725E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>8</v>
       </c>
@@ -4586,8 +4746,12 @@
       <c r="F41" s="9">
         <v>4975659</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G41" s="15">
+        <f t="shared" si="0"/>
+        <v>8.4873005776246083E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>8</v>
       </c>
@@ -4607,8 +4771,12 @@
       <c r="F42" s="9">
         <v>11955320</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G42" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12719591404250416</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>8</v>
       </c>
@@ -4628,8 +4796,12 @@
       <c r="F43" s="9">
         <v>19360086</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G43" s="15">
+        <f t="shared" si="0"/>
+        <v>0.14112420118116059</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>8</v>
       </c>
@@ -4649,8 +4821,12 @@
       <c r="F44" s="9">
         <v>56036600</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G44" s="15">
+        <f t="shared" si="0"/>
+        <v>0.17153082011047849</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>9</v>
       </c>
@@ -4670,8 +4846,12 @@
       <c r="F45" s="9">
         <v>52543</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G45" s="15">
+        <f t="shared" si="0"/>
+        <v>7.0547127933147588E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>9</v>
       </c>
@@ -4691,8 +4871,12 @@
       <c r="F46" s="9">
         <v>1995433</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G46" s="15">
+        <f t="shared" si="0"/>
+        <v>7.4143778736091306E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>9</v>
       </c>
@@ -4712,8 +4896,12 @@
       <c r="F47" s="9">
         <v>5055150</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G47" s="15">
+        <f t="shared" si="0"/>
+        <v>0.1178350682934774</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>9</v>
       </c>
@@ -4733,8 +4921,12 @@
       <c r="F48" s="9">
         <v>8648376</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G48" s="15">
+        <f t="shared" si="0"/>
+        <v>0.13781226234871985</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>9</v>
       </c>
@@ -4754,8 +4946,12 @@
       <c r="F49" s="9">
         <v>20490270</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G49" s="15">
+        <f t="shared" si="0"/>
+        <v>0.16230520799894796</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>10</v>
       </c>
@@ -4775,8 +4971,12 @@
       <c r="F50" s="9">
         <v>61210</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G50" s="15">
+        <f t="shared" si="0"/>
+        <v>4.8960757724717356E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>10</v>
       </c>
@@ -4796,8 +4996,12 @@
       <c r="F51" s="9">
         <v>2670510</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G51" s="15">
+        <f t="shared" si="0"/>
+        <v>5.0492989734977178E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>10</v>
       </c>
@@ -4817,8 +5021,12 @@
       <c r="F52" s="9">
         <v>9009274</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G52" s="15">
+        <f t="shared" si="0"/>
+        <v>0.10313247141065728</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>10</v>
       </c>
@@ -4838,8 +5046,12 @@
       <c r="F53" s="9">
         <v>15263065</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G53" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12444453724725812</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>10</v>
       </c>
@@ -4859,8 +5071,12 @@
       <c r="F54" s="9">
         <v>34511574</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G54" s="15">
+        <f t="shared" si="0"/>
+        <v>0.15072532084140183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>11</v>
       </c>
@@ -4880,8 +5096,12 @@
       <c r="F55" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G55" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>11</v>
       </c>
@@ -4901,8 +5121,12 @@
       <c r="F56" s="9">
         <v>1645353</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G56" s="15">
+        <f t="shared" si="0"/>
+        <v>3.3070320898806814E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>11</v>
       </c>
@@ -4922,8 +5146,12 @@
       <c r="F57" s="9">
         <v>8724984</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G57" s="15">
+        <f t="shared" si="0"/>
+        <v>9.538600902785134E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>11</v>
       </c>
@@ -4943,8 +5171,12 @@
       <c r="F58" s="9">
         <v>16556794</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G58" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12180006746499707</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>11</v>
       </c>
@@ -4964,8 +5196,12 @@
       <c r="F59" s="9">
         <v>44800611</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G59" s="15">
+        <f t="shared" si="0"/>
+        <v>0.15828013888935161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>12</v>
       </c>
@@ -4985,8 +5221,12 @@
       <c r="F60" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G60" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>12</v>
       </c>
@@ -5006,8 +5246,12 @@
       <c r="F61" s="9">
         <v>234228</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G61" s="15">
+        <f>F61/E61</f>
+        <v>3.2772329356957002E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>12</v>
       </c>
@@ -5027,8 +5271,12 @@
       <c r="F62" s="9">
         <v>1426677</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G62" s="15">
+        <f t="shared" si="0"/>
+        <v>0.10588558798731758</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>12</v>
       </c>
@@ -5048,8 +5296,12 @@
       <c r="F63" s="9">
         <v>3021298</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G63" s="15">
+        <f t="shared" si="0"/>
+        <v>0.14241857569734026</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>12</v>
       </c>
@@ -5069,8 +5321,12 @@
       <c r="F64" s="9">
         <v>9190695</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G64" s="15">
+        <f t="shared" si="0"/>
+        <v>0.17019741889113674</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>13</v>
       </c>
@@ -5090,8 +5346,12 @@
       <c r="F65" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G65" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>13</v>
       </c>
@@ -5111,8 +5371,12 @@
       <c r="F66" s="9">
         <v>393258</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G66" s="15">
+        <f t="shared" si="0"/>
+        <v>3.4994904151508077E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>13</v>
       </c>
@@ -5132,8 +5396,12 @@
       <c r="F67" s="9">
         <v>1834009</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G67" s="15">
+        <f t="shared" si="0"/>
+        <v>9.2546001166962003E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>13</v>
       </c>
@@ -5153,8 +5421,12 @@
       <c r="F68" s="9">
         <v>3659633</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G68" s="15">
+        <f t="shared" si="0"/>
+        <v>0.12488673752754609</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>13</v>
       </c>
@@ -5174,8 +5446,12 @@
       <c r="F69" s="9">
         <v>9051372</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G69" s="15">
+        <f t="shared" si="0"/>
+        <v>0.15547858079844754</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>14</v>
       </c>
@@ -5195,8 +5471,12 @@
       <c r="F70" s="9">
         <v>24484</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G70" s="15">
+        <f t="shared" ref="G70:G77" si="1">F70/E70</f>
+        <v>4.0317421476618156E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>14</v>
       </c>
@@ -5216,8 +5496,12 @@
       <c r="F71" s="9">
         <v>1972651</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G71" s="15">
+        <f t="shared" si="1"/>
+        <v>8.2902023654749191E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>14</v>
       </c>
@@ -5237,8 +5521,12 @@
       <c r="F72" s="9">
         <v>4743479</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G72" s="15">
+        <f t="shared" si="1"/>
+        <v>0.12574560968665652</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>14</v>
       </c>
@@ -5258,8 +5546,12 @@
       <c r="F73" s="9">
         <v>7858972</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G73" s="15">
+        <f t="shared" si="1"/>
+        <v>0.14412750666117566</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>14</v>
       </c>
@@ -5279,8 +5571,12 @@
       <c r="F74" s="9">
         <v>22616293</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G74" s="15">
+        <f t="shared" si="1"/>
+        <v>0.17157256232806931</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>15</v>
       </c>
@@ -5300,8 +5596,12 @@
       <c r="F75" s="9">
         <v>32877</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G75" s="15">
+        <f t="shared" si="1"/>
+        <v>3.5270195638712701E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>15</v>
       </c>
@@ -5321,8 +5621,12 @@
       <c r="F76" s="9">
         <v>2618620</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G76" s="15">
+        <f t="shared" si="1"/>
+        <v>7.3772623894366382E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>15</v>
       </c>
@@ -5342,8 +5646,12 @@
       <c r="F77" s="9">
         <v>6052843</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G77" s="15">
+        <f t="shared" si="1"/>
+        <v>0.11138748814625489</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>15</v>
       </c>
@@ -5363,8 +5671,12 @@
       <c r="F78" s="9">
         <v>9529943</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G78" s="15">
+        <f>F78/E78</f>
+        <v>0.12606418218560644</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>15</v>
       </c>
@@ -5384,8 +5696,12 @@
       <c r="F79" s="9">
         <v>21580220</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G79" s="15">
+        <f t="shared" ref="G79:G100" si="2">F79/E79</f>
+        <v>0.15493218235929285</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>16</v>
       </c>
@@ -5405,8 +5721,12 @@
       <c r="F80" s="9">
         <v>21249</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G80" s="15">
+        <f t="shared" si="2"/>
+        <v>7.3940324392338516E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>16</v>
       </c>
@@ -5426,8 +5746,12 @@
       <c r="F81" s="9">
         <v>583802</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G81" s="15">
+        <f t="shared" si="2"/>
+        <v>3.8567398478013319E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>16</v>
       </c>
@@ -5447,8 +5771,12 @@
       <c r="F82" s="9">
         <v>2643853</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G82" s="15">
+        <f t="shared" si="2"/>
+        <v>9.7658972455240231E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>16</v>
       </c>
@@ -5468,8 +5796,12 @@
       <c r="F83" s="9">
         <v>4702754</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G83" s="15">
+        <f t="shared" si="2"/>
+        <v>0.12090827613264561</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>16</v>
       </c>
@@ -5489,8 +5821,12 @@
       <c r="F84" s="9">
         <v>12263342</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G84" s="15">
+        <f t="shared" si="2"/>
+        <v>0.15412337270246421</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>17</v>
       </c>
@@ -5510,8 +5846,12 @@
       <c r="F85" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G85" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>17</v>
       </c>
@@ -5531,8 +5871,12 @@
       <c r="F86" s="9">
         <v>799087</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G86" s="15">
+        <f t="shared" si="2"/>
+        <v>2.1678092906639527E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>17</v>
       </c>
@@ -5552,8 +5896,12 @@
       <c r="F87" s="9">
         <v>6051723</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G87" s="15">
+        <f t="shared" si="2"/>
+        <v>8.7043329540762993E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>17</v>
       </c>
@@ -5573,8 +5921,12 @@
       <c r="F88" s="9">
         <v>12729152</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G88" s="15">
+        <f t="shared" si="2"/>
+        <v>0.12023870588387207</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>17</v>
       </c>
@@ -5594,8 +5946,12 @@
       <c r="F89" s="9">
         <v>37568246</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G89" s="15">
+        <f t="shared" si="2"/>
+        <v>0.1603933303025534</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>18</v>
       </c>
@@ -5615,8 +5971,12 @@
       <c r="F90" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G90" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>18</v>
       </c>
@@ -5636,8 +5996,12 @@
       <c r="F91" s="9">
         <v>382611</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G91" s="15">
+        <f t="shared" si="2"/>
+        <v>2.2372650157185862E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>18</v>
       </c>
@@ -5657,8 +6021,12 @@
       <c r="F92" s="9">
         <v>2550599</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G92" s="15">
+        <f t="shared" si="2"/>
+        <v>8.360159318359292E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>18</v>
       </c>
@@ -5678,8 +6046,12 @@
       <c r="F93" s="9">
         <v>4555972</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G93" s="15">
+        <f t="shared" si="2"/>
+        <v>0.10290798846691611</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>18</v>
       </c>
@@ -5699,8 +6071,12 @@
       <c r="F94" s="9">
         <v>10773948</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G94" s="15">
+        <f t="shared" si="2"/>
+        <v>0.13827331931299622</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>19</v>
       </c>
@@ -5720,8 +6096,12 @@
       <c r="F95" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G95" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>19</v>
       </c>
@@ -5741,8 +6121,12 @@
       <c r="F96" s="9">
         <v>263755</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G96" s="15">
+        <f t="shared" si="2"/>
+        <v>3.400194609913864E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>19</v>
       </c>
@@ -5762,8 +6146,12 @@
       <c r="F97" s="9">
         <v>1145092</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G97" s="15">
+        <f t="shared" si="2"/>
+        <v>8.5497464923843192E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>19</v>
       </c>
@@ -5783,8 +6171,12 @@
       <c r="F98" s="9">
         <v>1998744</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G98" s="15">
+        <f t="shared" si="2"/>
+        <v>0.10587816127049725</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>19</v>
       </c>
@@ -5804,8 +6196,12 @@
       <c r="F99" s="9">
         <v>4490346</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G99" s="15">
+        <f t="shared" si="2"/>
+        <v>0.13891922549929803</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>20</v>
       </c>
@@ -5825,8 +6221,12 @@
       <c r="F100" s="9">
         <v>171673</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G100" s="15">
+        <f t="shared" si="2"/>
+        <v>8.4560473991422049E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>20</v>
       </c>
@@ -5846,8 +6246,12 @@
       <c r="F101" s="9">
         <v>7420987</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G101" s="15">
+        <f>F101/E101</f>
+        <v>8.3117149218135178E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>20</v>
       </c>
@@ -5867,8 +6271,12 @@
       <c r="F102" s="9">
         <v>17880919</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G102" s="15">
+        <f t="shared" ref="G102:G111" si="3">F102/E102</f>
+        <v>0.11946408147566101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>20</v>
       </c>
@@ -5888,8 +6296,12 @@
       <c r="F103" s="9">
         <v>30918010</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G103" s="15">
+        <f t="shared" si="3"/>
+        <v>0.1363638705210693</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>20</v>
       </c>
@@ -5909,8 +6321,12 @@
       <c r="F104" s="9">
         <v>101504376</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G104" s="15">
+        <f t="shared" si="3"/>
+        <v>0.17428568207920689</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>30</v>
       </c>
@@ -5930,8 +6346,12 @@
       <c r="F105" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G105" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>30</v>
       </c>
@@ -5951,8 +6371,12 @@
       <c r="F106" s="9">
         <v>324794</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G106" s="15">
+        <f t="shared" si="3"/>
+        <v>7.1937786840058832E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>30</v>
       </c>
@@ -5972,8 +6396,12 @@
       <c r="F107" s="9">
         <v>1019910</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G107" s="15">
+        <f t="shared" si="3"/>
+        <v>0.11815623857432614</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>30</v>
       </c>
@@ -5993,8 +6421,12 @@
       <c r="F108" s="9">
         <v>1904172</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G108" s="15">
+        <f t="shared" si="3"/>
+        <v>0.13445148642674562</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>30</v>
       </c>
@@ -6014,8 +6446,15 @@
       <c r="F109" s="9">
         <v>8974933</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G109" s="15">
+        <f t="shared" si="3"/>
+        <v>0.18457543692468331</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G110" s="15"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C111" t="s">
         <v>20</v>
       </c>
@@ -6030,6 +6469,10 @@
       <c r="F111" s="2">
         <f>SUM(F5:F109)</f>
         <v>1115105002</v>
+      </c>
+      <c r="G111" s="15">
+        <f t="shared" si="3"/>
+        <v>0.14161095500776338</v>
       </c>
     </row>
   </sheetData>
@@ -6041,7 +6484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -8739,7 +9182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3922145D-3645-6845-8B66-A062D36AF928}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+    <sheetView zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -9008,10 +9451,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94E1ACB-C1A3-994E-AE99-9A35AAA9A062}">
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9024,17 +9467,17 @@
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -9053,8 +9496,11 @@
       <c r="F4" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G4" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -9074,8 +9520,12 @@
       <c r="F5" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G5" s="15">
+        <f>F5/E5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -9095,8 +9545,12 @@
       <c r="F6" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G6" s="15">
+        <f t="shared" ref="G6:G69" si="0">F6/E6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -9116,8 +9570,12 @@
       <c r="F7" s="9">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G7" s="15">
+        <f t="shared" si="0"/>
+        <v>5.7433504459838309E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -9137,8 +9595,12 @@
       <c r="F8" s="9">
         <v>104183</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G8" s="15">
+        <f t="shared" si="0"/>
+        <v>1.7812304104277454E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -9158,8 +9620,12 @@
       <c r="F9" s="9">
         <v>9132731</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G9" s="15">
+        <f t="shared" si="0"/>
+        <v>5.6128783983828432E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -9179,8 +9645,12 @@
       <c r="F10" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G10" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -9200,8 +9670,12 @@
       <c r="F11" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -9221,8 +9695,12 @@
       <c r="F12" s="9">
         <v>1763</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G12" s="15">
+        <f t="shared" si="0"/>
+        <v>6.1569862463823347E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -9242,8 +9720,12 @@
       <c r="F13" s="9">
         <v>268160</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G13" s="15">
+        <f t="shared" si="0"/>
+        <v>2.0451983964473097E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -9263,8 +9745,12 @@
       <c r="F14" s="9">
         <v>18221629</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G14" s="15">
+        <f t="shared" si="0"/>
+        <v>4.5412400886152299E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>3</v>
       </c>
@@ -9284,8 +9770,12 @@
       <c r="F15" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G15" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
@@ -9305,8 +9795,12 @@
       <c r="F16" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G16" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -9326,8 +9820,12 @@
       <c r="F17" s="9">
         <v>207</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G17" s="15">
+        <f t="shared" si="0"/>
+        <v>4.2745156741430565E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
@@ -9347,8 +9845,12 @@
       <c r="F18" s="9">
         <v>370114</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G18" s="15">
+        <f t="shared" si="0"/>
+        <v>1.6688975885621612E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3</v>
       </c>
@@ -9368,8 +9870,12 @@
       <c r="F19" s="9">
         <v>12487875</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G19" s="15">
+        <f t="shared" si="0"/>
+        <v>5.1196971280181537E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>4</v>
       </c>
@@ -9389,8 +9895,12 @@
       <c r="F20" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G20" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>4</v>
       </c>
@@ -9410,8 +9920,12 @@
       <c r="F21" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G21" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>4</v>
       </c>
@@ -9431,8 +9945,12 @@
       <c r="F22" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G22" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>4</v>
       </c>
@@ -9452,8 +9970,12 @@
       <c r="F23" s="9">
         <v>20675</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G23" s="15">
+        <f t="shared" si="0"/>
+        <v>2.7742635615060336E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>4</v>
       </c>
@@ -9473,8 +9995,12 @@
       <c r="F24" s="9">
         <v>2798970</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G24" s="15">
+        <f t="shared" si="0"/>
+        <v>4.1292118805399741E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>5</v>
       </c>
@@ -9494,8 +10020,12 @@
       <c r="F25" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G25" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>5</v>
       </c>
@@ -9515,8 +10045,12 @@
       <c r="F26" s="9">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G26" s="15">
+        <f t="shared" si="0"/>
+        <v>1.8896480070498659E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>5</v>
       </c>
@@ -9536,8 +10070,12 @@
       <c r="F27" s="9">
         <v>15978</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G27" s="15">
+        <f t="shared" si="0"/>
+        <v>2.049063043544975E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>5</v>
       </c>
@@ -9557,8 +10095,12 @@
       <c r="F28" s="9">
         <v>757059</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G28" s="15">
+        <f t="shared" si="0"/>
+        <v>2.2891985276949998E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>5</v>
       </c>
@@ -9578,8 +10120,12 @@
       <c r="F29" s="9">
         <v>36467745</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G29" s="15">
+        <f t="shared" si="0"/>
+        <v>5.8482501743054305E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>6</v>
       </c>
@@ -9599,8 +10145,12 @@
       <c r="F30" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G30" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>6</v>
       </c>
@@ -9620,8 +10170,12 @@
       <c r="F31" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G31" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>6</v>
       </c>
@@ -9641,8 +10195,12 @@
       <c r="F32" s="9">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G32" s="15">
+        <f t="shared" si="0"/>
+        <v>6.3011332588165983E-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>6</v>
       </c>
@@ -9662,8 +10220,12 @@
       <c r="F33" s="9">
         <v>25993</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G33" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9288836987614249E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>6</v>
       </c>
@@ -9683,8 +10245,12 @@
       <c r="F34" s="9">
         <v>6353278</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G34" s="15">
+        <f t="shared" si="0"/>
+        <v>4.2032045366699302E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>7</v>
       </c>
@@ -9704,8 +10270,12 @@
       <c r="F35" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G35" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>7</v>
       </c>
@@ -9725,8 +10295,12 @@
       <c r="F36" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G36" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>7</v>
       </c>
@@ -9746,8 +10320,12 @@
       <c r="F37" s="9">
         <v>22069</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G37" s="15">
+        <f t="shared" si="0"/>
+        <v>3.1891170085137385E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>7</v>
       </c>
@@ -9767,8 +10345,12 @@
       <c r="F38" s="9">
         <v>803083</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G38" s="15">
+        <f t="shared" si="0"/>
+        <v>2.5705490534694581E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>7</v>
       </c>
@@ -9788,8 +10370,12 @@
       <c r="F39" s="9">
         <v>89278854</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G39" s="15">
+        <f t="shared" si="0"/>
+        <v>7.3360505703490659E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>8</v>
       </c>
@@ -9809,8 +10395,12 @@
       <c r="F40" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G40" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>8</v>
       </c>
@@ -9830,8 +10420,12 @@
       <c r="F41" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G41" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>8</v>
       </c>
@@ -9851,8 +10445,12 @@
       <c r="F42" s="9">
         <v>65</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G42" s="15">
+        <f t="shared" si="0"/>
+        <v>1.0102491485775599E-6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>8</v>
       </c>
@@ -9872,8 +10470,12 @@
       <c r="F43" s="9">
         <v>495230</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G43" s="15">
+        <f t="shared" si="0"/>
+        <v>1.6746077218815498E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>8</v>
       </c>
@@ -9893,8 +10495,12 @@
       <c r="F44" s="9">
         <v>14735916</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G44" s="15">
+        <f t="shared" si="0"/>
+        <v>4.9373449118175873E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>9</v>
       </c>
@@ -9914,8 +10520,12 @@
       <c r="F45" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G45" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>9</v>
       </c>
@@ -9935,8 +10545,12 @@
       <c r="F46" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G46" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>9</v>
       </c>
@@ -9956,8 +10570,12 @@
       <c r="F47" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G47" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>9</v>
       </c>
@@ -9977,8 +10595,12 @@
       <c r="F48" s="9">
         <v>122274</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G48" s="15">
+        <f t="shared" si="0"/>
+        <v>1.1473347615418199E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>9</v>
       </c>
@@ -9998,8 +10620,12 @@
       <c r="F49" s="9">
         <v>3911098</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G49" s="15">
+        <f t="shared" si="0"/>
+        <v>4.7231351432348309E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>10</v>
       </c>
@@ -10019,8 +10645,12 @@
       <c r="F50" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G50" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>10</v>
       </c>
@@ -10040,8 +10670,12 @@
       <c r="F51" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G51" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>10</v>
       </c>
@@ -10061,8 +10695,12 @@
       <c r="F52" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G52" s="15">
+        <f t="shared" si="0"/>
+        <v>3.1016362785575405E-7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>10</v>
       </c>
@@ -10082,8 +10720,12 @@
       <c r="F53" s="9">
         <v>18437</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G53" s="15">
+        <f t="shared" si="0"/>
+        <v>1.7294159078573359E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>10</v>
       </c>
@@ -10103,8 +10745,12 @@
       <c r="F54" s="9">
         <v>4346933</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G54" s="15">
+        <f t="shared" si="0"/>
+        <v>3.8138688719468439E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>11</v>
       </c>
@@ -10124,8 +10770,12 @@
       <c r="F55" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G55" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>11</v>
       </c>
@@ -10145,8 +10795,12 @@
       <c r="F56" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G56" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>11</v>
       </c>
@@ -10166,8 +10820,12 @@
       <c r="F57" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G57" s="15">
+        <f t="shared" si="0"/>
+        <v>2.8842814735678679E-7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>11</v>
       </c>
@@ -10187,8 +10845,12 @@
       <c r="F58" s="9">
         <v>9739</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G58" s="15">
+        <f t="shared" si="0"/>
+        <v>9.3630122330316934E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>11</v>
       </c>
@@ -10208,8 +10870,12 @@
       <c r="F59" s="9">
         <v>5545306</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G59" s="15">
+        <f t="shared" si="0"/>
+        <v>4.2171585773557747E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>12</v>
       </c>
@@ -10229,8 +10895,12 @@
       <c r="F60" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G60" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>12</v>
       </c>
@@ -10250,8 +10920,12 @@
       <c r="F61" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G61" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>12</v>
       </c>
@@ -10271,8 +10945,12 @@
       <c r="F62" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G62" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>12</v>
       </c>
@@ -10292,8 +10970,12 @@
       <c r="F63" s="9">
         <v>4037</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G63" s="15">
+        <f t="shared" si="0"/>
+        <v>2.214009431230465E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>12</v>
       </c>
@@ -10313,8 +10995,12 @@
       <c r="F64" s="9">
         <v>1780144</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G64" s="15">
+        <f t="shared" si="0"/>
+        <v>4.7608732845958656E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>13</v>
       </c>
@@ -10334,8 +11020,12 @@
       <c r="F65" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G65" s="15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>13</v>
       </c>
@@ -10355,8 +11045,12 @@
       <c r="F66" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G66" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>13</v>
       </c>
@@ -10376,8 +11070,12 @@
       <c r="F67" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G67" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>13</v>
       </c>
@@ -10397,8 +11095,12 @@
       <c r="F68" s="9">
         <v>1482</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G68" s="15">
+        <f t="shared" si="0"/>
+        <v>6.6643268074344561E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>13</v>
       </c>
@@ -10418,8 +11120,12 @@
       <c r="F69" s="9">
         <v>1237522</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G69" s="15">
+        <f t="shared" si="0"/>
+        <v>4.262520759054274E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>14</v>
       </c>
@@ -10439,8 +11145,12 @@
       <c r="F70" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G70" s="15">
+        <f t="shared" ref="G70:G111" si="1">F70/E70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>14</v>
       </c>
@@ -10460,8 +11170,12 @@
       <c r="F71" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G71" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>14</v>
       </c>
@@ -10481,8 +11195,12 @@
       <c r="F72" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G72" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>14</v>
       </c>
@@ -10502,8 +11220,12 @@
       <c r="F73" s="9">
         <v>109779</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G73" s="15">
+        <f t="shared" si="1"/>
+        <v>1.1958031306689991E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>14</v>
       </c>
@@ -10523,8 +11245,12 @@
       <c r="F74" s="9">
         <v>4481771</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G74" s="15">
+        <f t="shared" si="1"/>
+        <v>4.9406336169136996E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>15</v>
       </c>
@@ -10544,8 +11270,12 @@
       <c r="F75" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G75" s="15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>15</v>
       </c>
@@ -10565,8 +11295,12 @@
       <c r="F76" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G76" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>15</v>
       </c>
@@ -10586,8 +11320,12 @@
       <c r="F77" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G77" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>15</v>
       </c>
@@ -10607,8 +11345,12 @@
       <c r="F78" s="9">
         <v>41074</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G78" s="15">
+        <f t="shared" si="1"/>
+        <v>4.5276582832088507E-4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>15</v>
       </c>
@@ -10628,8 +11370,12 @@
       <c r="F79" s="9">
         <v>3849474</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G79" s="15">
+        <f t="shared" si="1"/>
+        <v>4.410926084030535E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>16</v>
       </c>
@@ -10649,8 +11395,12 @@
       <c r="F80" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G80" s="15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>16</v>
       </c>
@@ -10670,8 +11420,12 @@
       <c r="F81" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G81" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>16</v>
       </c>
@@ -10691,8 +11445,12 @@
       <c r="F82" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G82" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>16</v>
       </c>
@@ -10712,8 +11470,12 @@
       <c r="F83" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G83" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>16</v>
       </c>
@@ -10733,8 +11495,12 @@
       <c r="F84" s="9">
         <v>802570</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G84" s="15">
+        <f t="shared" si="1"/>
+        <v>3.5735086109393069E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>17</v>
       </c>
@@ -10754,8 +11520,12 @@
       <c r="F85" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G85" s="15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>17</v>
       </c>
@@ -10775,8 +11545,12 @@
       <c r="F86" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G86" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>17</v>
       </c>
@@ -10796,8 +11570,12 @@
       <c r="F87" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G87" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>17</v>
       </c>
@@ -10817,8 +11595,12 @@
       <c r="F88" s="9">
         <v>1519</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G88" s="15">
+        <f t="shared" si="1"/>
+        <v>2.2012394876685375E-5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>17</v>
       </c>
@@ -10838,8 +11620,12 @@
       <c r="F89" s="9">
         <v>4448137</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G89" s="15">
+        <f t="shared" si="1"/>
+        <v>4.0982564194590601E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>18</v>
       </c>
@@ -10859,8 +11645,12 @@
       <c r="F90" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G90" s="15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>18</v>
       </c>
@@ -10880,8 +11670,12 @@
       <c r="F91" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G91" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>18</v>
       </c>
@@ -10901,8 +11695,12 @@
       <c r="F92" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G92" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>18</v>
       </c>
@@ -10922,8 +11720,12 @@
       <c r="F93" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G93" s="15">
+        <f t="shared" si="1"/>
+        <v>3.5909007436970894E-7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>18</v>
       </c>
@@ -10943,8 +11745,12 @@
       <c r="F94" s="9">
         <v>760885</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G94" s="15">
+        <f t="shared" si="1"/>
+        <v>3.3523140730376973E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>19</v>
       </c>
@@ -10964,8 +11770,12 @@
       <c r="F95" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G95" s="15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>19</v>
       </c>
@@ -10985,8 +11795,12 @@
       <c r="F96" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G96" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>19</v>
       </c>
@@ -11006,8 +11820,12 @@
       <c r="F97" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G97" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>19</v>
       </c>
@@ -11027,8 +11845,12 @@
       <c r="F98" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G98" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>19</v>
       </c>
@@ -11048,8 +11870,12 @@
       <c r="F99" s="9">
         <v>332839</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G99" s="15">
+        <f t="shared" si="1"/>
+        <v>3.3042082182389823E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>20</v>
       </c>
@@ -11069,8 +11895,12 @@
       <c r="F100" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G100" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>20</v>
       </c>
@@ -11090,8 +11920,12 @@
       <c r="F101" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G101" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>20</v>
       </c>
@@ -11111,8 +11945,12 @@
       <c r="F102" s="9">
         <v>13308</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G102" s="15">
+        <f t="shared" si="1"/>
+        <v>1.0879922122387319E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>20</v>
       </c>
@@ -11132,8 +11970,12 @@
       <c r="F103" s="9">
         <v>1327597</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G103" s="15">
+        <f t="shared" si="1"/>
+        <v>2.2226857720479306E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>20</v>
       </c>
@@ -11153,8 +11995,12 @@
       <c r="F104" s="9">
         <v>34825649</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G104" s="15">
+        <f t="shared" si="1"/>
+        <v>5.1059861866586051E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>30</v>
       </c>
@@ -11174,8 +12020,12 @@
       <c r="F105" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G105" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>30</v>
       </c>
@@ -11195,8 +12045,12 @@
       <c r="F106" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G106" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>30</v>
       </c>
@@ -11216,8 +12070,12 @@
       <c r="F107" s="9">
         <v>6090</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G107" s="15">
+        <f t="shared" si="1"/>
+        <v>5.6208604992874706E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>30</v>
       </c>
@@ -11237,8 +12095,12 @@
       <c r="F108" s="9">
         <v>149605</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G108" s="15">
+        <f t="shared" si="1"/>
+        <v>2.9241036538991787E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>30</v>
       </c>
@@ -11258,8 +12120,15 @@
       <c r="F109" s="9">
         <v>9597244</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G109" s="15">
+        <f t="shared" si="1"/>
+        <v>6.764383636899904E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G110" s="15"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C111" t="s">
         <v>20</v>
       </c>
@@ -11274,6 +12143,10 @@
       <c r="F111" s="2">
         <f>SUM(F5:F109)</f>
         <v>270086215</v>
+      </c>
+      <c r="G111" s="15">
+        <f t="shared" si="1"/>
+        <v>5.316448521327951E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>